<commit_message>
MY change for MAP and adding WHA, ACTY
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\PycharmProjects\Release-Team-Verification-Suite\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044115A6-D062-4DFC-95C2-20BD6A044E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CF3BCB-1ED8-4BBC-A753-D738261047AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="172">
   <si>
     <t>Customer Name</t>
   </si>
@@ -535,6 +535,12 @@
   </si>
   <si>
     <t>scmg_ali.alamar</t>
+  </si>
+  <si>
+    <t>AllCare To You</t>
+  </si>
+  <si>
+    <t>Western Health Advantage</t>
   </si>
 </sst>
 </file>
@@ -690,7 +696,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -747,6 +753,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1064,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H117" sqref="H117"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1139,16 +1148,16 @@
     </row>
     <row r="5" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>7</v>
+        <v>170</v>
       </c>
       <c r="B5" s="10">
-        <v>1500</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>136</v>
+        <v>1750</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3">
+        <v>99999</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -1159,11 +1168,11 @@
       <c r="B6" s="10">
         <v>1500</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>137</v>
+      <c r="C6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -1174,11 +1183,11 @@
       <c r="B7" s="10">
         <v>1500</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>138</v>
+      <c r="C7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -1189,26 +1198,26 @@
       <c r="B8" s="10">
         <v>1500</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>6</v>
+      <c r="C8" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="10">
-        <v>3700</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>5</v>
+        <v>1500</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -1219,35 +1228,35 @@
       <c r="B10" s="10">
         <v>3700</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>9</v>
+      <c r="C10" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="10">
-        <v>2200</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="10">
-        <v>99999</v>
+        <v>3700</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>132</v>
+        <v>11</v>
       </c>
       <c r="B12" s="10">
-        <v>6800</v>
+        <v>2200</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>12</v>
@@ -1259,16 +1268,16 @@
     </row>
     <row r="13" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>13</v>
+        <v>132</v>
       </c>
       <c r="B13" s="10">
-        <v>1600</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>60</v>
+        <v>6800</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="10">
+        <v>99999</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -1279,11 +1288,11 @@
       <c r="B14" s="10">
         <v>1600</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>8</v>
+      <c r="C14" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -1294,11 +1303,11 @@
       <c r="B15" s="10">
         <v>1600</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>9</v>
+      <c r="C15" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1"/>
     </row>
@@ -1309,11 +1318,11 @@
       <c r="B16" s="10">
         <v>1600</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>14</v>
+      <c r="C16" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -1324,86 +1333,86 @@
       <c r="B17" s="10">
         <v>1600</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>6</v>
+      <c r="C17" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>131</v>
+        <v>13</v>
       </c>
       <c r="B18" s="10">
-        <v>6700</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="10">
-        <v>99999</v>
+        <v>1600</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="10">
+        <v>6700</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="10">
+        <v>99999</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B20" s="10">
         <v>7100</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C20" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="10">
-        <v>4700</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="10">
-        <v>99999</v>
       </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="10">
+        <v>4700</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="10">
+        <v>99999</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B22" s="10">
         <v>7500</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="10">
-        <v>3200</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>65</v>
+      <c r="D22" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -1414,11 +1423,11 @@
       <c r="B23" s="10">
         <v>3200</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>8</v>
+      <c r="C23" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23" s="1"/>
     </row>
@@ -1429,26 +1438,26 @@
       <c r="B24" s="10">
         <v>3200</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>67</v>
+      <c r="C24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" s="10">
-        <v>3100</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>5</v>
+        <v>3200</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E25" s="1"/>
     </row>
@@ -1459,26 +1468,26 @@
       <c r="B26" s="10">
         <v>3100</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>8</v>
+      <c r="C26" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="10">
-        <v>1700</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>70</v>
+        <v>3100</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="E27" s="1"/>
     </row>
@@ -1489,11 +1498,11 @@
       <c r="B28" s="10">
         <v>1700</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>8</v>
+      <c r="C28" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E28" s="1"/>
     </row>
@@ -1504,26 +1513,26 @@
       <c r="B29" s="10">
         <v>1700</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>9</v>
+      <c r="C29" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" s="10">
-        <v>2900</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>5</v>
+        <v>1700</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="E30" s="1"/>
     </row>
@@ -1534,11 +1543,11 @@
       <c r="B31" s="10">
         <v>2900</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>14</v>
+      <c r="C31" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E31" s="1"/>
     </row>
@@ -1549,26 +1558,26 @@
       <c r="B32" s="10">
         <v>2900</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>6</v>
+      <c r="C32" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B33" s="10">
-        <v>1800</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>5</v>
+        <v>2900</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="E33" s="1"/>
     </row>
@@ -1579,11 +1588,11 @@
       <c r="B34" s="10">
         <v>1800</v>
       </c>
-      <c r="C34" s="14" t="s">
-        <v>8</v>
+      <c r="C34" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E34" s="1"/>
     </row>
@@ -1594,11 +1603,11 @@
       <c r="B35" s="10">
         <v>1800</v>
       </c>
-      <c r="C35" s="16" t="s">
-        <v>14</v>
+      <c r="C35" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E35" s="1"/>
     </row>
@@ -1609,41 +1618,41 @@
       <c r="B36" s="10">
         <v>1800</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>6</v>
+      <c r="C36" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B37" s="10">
-        <v>4300</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>140</v>
+        <v>1800</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" s="10">
-        <v>3000</v>
+        <v>4300</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="17" t="s">
-        <v>77</v>
+      <c r="D38" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="E38" s="1"/>
     </row>
@@ -1654,11 +1663,11 @@
       <c r="B39" s="10">
         <v>3000</v>
       </c>
-      <c r="C39" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>141</v>
+      <c r="C39" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="E39" s="1"/>
     </row>
@@ -1669,11 +1678,11 @@
       <c r="B40" s="10">
         <v>3000</v>
       </c>
-      <c r="C40" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>142</v>
+      <c r="C40" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="E40" s="1"/>
     </row>
@@ -1684,11 +1693,11 @@
       <c r="B41" s="10">
         <v>3000</v>
       </c>
-      <c r="C41" s="16" t="s">
-        <v>14</v>
+      <c r="C41" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E41" s="1"/>
     </row>
@@ -1699,26 +1708,26 @@
       <c r="B42" s="10">
         <v>3000</v>
       </c>
-      <c r="C42" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>78</v>
+      <c r="C42" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B43" s="10">
-        <v>3500</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>79</v>
+        <v>3000</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="E43" s="1"/>
     </row>
@@ -1729,11 +1738,11 @@
       <c r="B44" s="10">
         <v>3500</v>
       </c>
-      <c r="C44" s="14" t="s">
-        <v>8</v>
+      <c r="C44" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E44" s="1"/>
     </row>
@@ -1744,35 +1753,35 @@
       <c r="B45" s="10">
         <v>3500</v>
       </c>
-      <c r="C45" s="16" t="s">
-        <v>14</v>
+      <c r="C45" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B46" s="10">
-        <v>200</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" s="10">
-        <v>99999</v>
+        <v>3500</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B47" s="10">
-        <v>3600</v>
+        <v>200</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>12</v>
@@ -1784,16 +1793,16 @@
     </row>
     <row r="48" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B48" s="10">
-        <v>4600</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>82</v>
+        <v>3600</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="10">
+        <v>99999</v>
       </c>
       <c r="E48" s="1"/>
     </row>
@@ -1804,11 +1813,11 @@
       <c r="B49" s="10">
         <v>4600</v>
       </c>
-      <c r="C49" s="14" t="s">
-        <v>8</v>
+      <c r="C49" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E49" s="1"/>
     </row>
@@ -1819,11 +1828,11 @@
       <c r="B50" s="10">
         <v>4600</v>
       </c>
-      <c r="C50" s="15" t="s">
-        <v>9</v>
+      <c r="C50" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E50" s="1"/>
     </row>
@@ -1834,26 +1843,26 @@
       <c r="B51" s="10">
         <v>4600</v>
       </c>
-      <c r="C51" s="13" t="s">
-        <v>6</v>
+      <c r="C51" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B52" s="10">
-        <v>150</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>5</v>
+        <v>4600</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E52" s="1"/>
     </row>
@@ -1864,11 +1873,11 @@
       <c r="B53" s="10">
         <v>150</v>
       </c>
-      <c r="C53" s="14" t="s">
-        <v>8</v>
+      <c r="C53" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E53" s="1"/>
     </row>
@@ -1879,11 +1888,11 @@
       <c r="B54" s="10">
         <v>150</v>
       </c>
-      <c r="C54" s="15" t="s">
-        <v>9</v>
+      <c r="C54" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E54" s="1"/>
     </row>
@@ -1894,11 +1903,11 @@
       <c r="B55" s="10">
         <v>150</v>
       </c>
-      <c r="C55" s="16" t="s">
-        <v>14</v>
+      <c r="C55" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E55" s="1"/>
     </row>
@@ -1909,26 +1918,26 @@
       <c r="B56" s="10">
         <v>150</v>
       </c>
-      <c r="C56" s="13" t="s">
-        <v>6</v>
+      <c r="C56" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B57" s="10">
-        <v>2700</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>165</v>
+        <v>150</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="E57" s="1"/>
     </row>
@@ -1939,35 +1948,35 @@
       <c r="B58" s="10">
         <v>2700</v>
       </c>
-      <c r="C58" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>150</v>
+      <c r="C58" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="10">
+        <v>2700</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B59" s="10">
+      <c r="B60" s="10">
         <v>2000</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59" s="10">
-        <v>99999</v>
-      </c>
-      <c r="E59" s="1"/>
-    </row>
-    <row r="60" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B60" s="10">
-        <v>2100</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>12</v>
@@ -1977,18 +1986,18 @@
       </c>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
-        <v>124</v>
+        <v>33</v>
       </c>
       <c r="B61" s="10">
-        <v>5600</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>125</v>
+        <v>2100</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="10">
+        <v>99999</v>
       </c>
       <c r="E61" s="1"/>
     </row>
@@ -1999,41 +2008,41 @@
       <c r="B62" s="10">
         <v>5600</v>
       </c>
-      <c r="C62" s="14" t="s">
-        <v>8</v>
+      <c r="C62" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="B63" s="10">
-        <v>2600</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D63" s="10">
-        <v>99999</v>
+        <v>5600</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B64" s="10">
-        <v>1100</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>85</v>
+        <v>2600</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="10">
+        <v>99999</v>
       </c>
       <c r="E64" s="1"/>
     </row>
@@ -2044,11 +2053,11 @@
       <c r="B65" s="10">
         <v>1100</v>
       </c>
-      <c r="C65" s="14" t="s">
-        <v>8</v>
+      <c r="C65" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E65" s="1"/>
     </row>
@@ -2059,11 +2068,11 @@
       <c r="B66" s="10">
         <v>1100</v>
       </c>
-      <c r="C66" s="15" t="s">
-        <v>9</v>
+      <c r="C66" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E66" s="1"/>
     </row>
@@ -2074,35 +2083,35 @@
       <c r="B67" s="10">
         <v>1100</v>
       </c>
-      <c r="C67" s="13" t="s">
-        <v>6</v>
+      <c r="C67" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B68" s="10">
-        <v>3300</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D68" s="10">
-        <v>99999</v>
+        <v>1100</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B69" s="10">
-        <v>5100</v>
+        <v>3300</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>12</v>
@@ -2114,10 +2123,10 @@
     </row>
     <row r="70" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B70" s="10">
-        <v>7400</v>
+        <v>5100</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>12</v>
@@ -2127,12 +2136,12 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
       <c r="B71" s="10">
-        <v>2800</v>
+        <v>7400</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>12</v>
@@ -2144,10 +2153,10 @@
     </row>
     <row r="72" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="B72" s="19">
-        <v>1550</v>
+        <v>158</v>
+      </c>
+      <c r="B72" s="10">
+        <v>2800</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>12</v>
@@ -2155,13 +2164,14 @@
       <c r="D72" s="10">
         <v>99999</v>
       </c>
+      <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="B73" s="10">
-        <v>6600</v>
+        <v>161</v>
+      </c>
+      <c r="B73" s="19">
+        <v>1550</v>
       </c>
       <c r="C73" s="11" t="s">
         <v>12</v>
@@ -2169,14 +2179,13 @@
       <c r="D73" s="10">
         <v>99999</v>
       </c>
-      <c r="E73" s="1"/>
     </row>
     <row r="74" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
-        <v>39</v>
+        <v>130</v>
       </c>
       <c r="B74" s="10">
-        <v>5200</v>
+        <v>6600</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>12</v>
@@ -2188,10 +2197,10 @@
     </row>
     <row r="75" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B75" s="10">
-        <v>4800</v>
+        <v>5200</v>
       </c>
       <c r="C75" s="11" t="s">
         <v>12</v>
@@ -2203,10 +2212,10 @@
     </row>
     <row r="76" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
-        <v>123</v>
+        <v>40</v>
       </c>
       <c r="B76" s="10">
-        <v>5300</v>
+        <v>4800</v>
       </c>
       <c r="C76" s="11" t="s">
         <v>12</v>
@@ -2218,10 +2227,10 @@
     </row>
     <row r="77" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="B77" s="10">
-        <v>4900</v>
+        <v>5300</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>12</v>
@@ -2231,12 +2240,12 @@
       </c>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B78" s="10">
-        <v>4100</v>
+        <v>4900</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>12</v>
@@ -2248,10 +2257,10 @@
     </row>
     <row r="79" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B79" s="10">
-        <v>5000</v>
+        <v>4100</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>12</v>
@@ -2263,10 +2272,10 @@
     </row>
     <row r="80" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="B80" s="19">
-        <v>1650</v>
+        <v>43</v>
+      </c>
+      <c r="B80" s="10">
+        <v>5000</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>12</v>
@@ -2274,13 +2283,14 @@
       <c r="D80" s="10">
         <v>99999</v>
       </c>
+      <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B81" s="10">
-        <v>4500</v>
+        <v>162</v>
+      </c>
+      <c r="B81" s="19">
+        <v>1650</v>
       </c>
       <c r="C81" s="11" t="s">
         <v>12</v>
@@ -2288,14 +2298,13 @@
       <c r="D81" s="10">
         <v>99999</v>
       </c>
-      <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B82" s="10">
-        <v>3400</v>
+        <v>4500</v>
       </c>
       <c r="C82" s="11" t="s">
         <v>12</v>
@@ -2307,16 +2316,16 @@
     </row>
     <row r="83" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B83" s="10">
-        <v>1200</v>
-      </c>
-      <c r="C83" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>89</v>
+        <v>3400</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83" s="10">
+        <v>99999</v>
       </c>
       <c r="E83" s="1"/>
     </row>
@@ -2327,11 +2336,11 @@
       <c r="B84" s="10">
         <v>1200</v>
       </c>
-      <c r="C84" s="12" t="s">
-        <v>5</v>
+      <c r="C84" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>166</v>
+        <v>89</v>
       </c>
       <c r="E84" s="1"/>
     </row>
@@ -2342,11 +2351,11 @@
       <c r="B85" s="10">
         <v>1200</v>
       </c>
-      <c r="C85" s="14" t="s">
-        <v>8</v>
+      <c r="C85" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
       <c r="E85" s="1"/>
     </row>
@@ -2357,26 +2366,26 @@
       <c r="B86" s="10">
         <v>1200</v>
       </c>
-      <c r="C86" s="15" t="s">
-        <v>9</v>
+      <c r="C86" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E86" s="1"/>
     </row>
     <row r="87" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B87" s="10">
-        <v>3900</v>
-      </c>
-      <c r="C87" s="12" t="s">
-        <v>5</v>
+        <v>1200</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E87" s="1"/>
     </row>
@@ -2387,11 +2396,11 @@
       <c r="B88" s="10">
         <v>3900</v>
       </c>
-      <c r="C88" s="15" t="s">
-        <v>9</v>
+      <c r="C88" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -2402,11 +2411,11 @@
       <c r="B89" s="10">
         <v>3900</v>
       </c>
-      <c r="C89" s="16" t="s">
-        <v>14</v>
+      <c r="C89" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E89" s="1"/>
     </row>
@@ -2417,26 +2426,26 @@
       <c r="B90" s="10">
         <v>3900</v>
       </c>
-      <c r="C90" s="13" t="s">
-        <v>6</v>
+      <c r="C90" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B91" s="10">
-        <v>3800</v>
-      </c>
-      <c r="C91" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>96</v>
+        <v>3900</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E91" s="1"/>
     </row>
@@ -2447,11 +2456,11 @@
       <c r="B92" s="10">
         <v>3800</v>
       </c>
-      <c r="C92" s="16" t="s">
-        <v>14</v>
+      <c r="C92" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E92" s="1"/>
     </row>
@@ -2462,26 +2471,26 @@
       <c r="B93" s="10">
         <v>3800</v>
       </c>
-      <c r="C93" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>164</v>
+      <c r="C93" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B94" s="10">
-        <v>1300</v>
-      </c>
-      <c r="C94" s="12" t="s">
-        <v>5</v>
+        <v>3800</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>98</v>
+        <v>164</v>
       </c>
       <c r="E94" s="1"/>
     </row>
@@ -2492,11 +2501,11 @@
       <c r="B95" s="10">
         <v>1300</v>
       </c>
-      <c r="C95" s="14" t="s">
-        <v>8</v>
+      <c r="C95" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E95" s="1"/>
     </row>
@@ -2507,11 +2516,11 @@
       <c r="B96" s="10">
         <v>1300</v>
       </c>
-      <c r="C96" s="15" t="s">
-        <v>9</v>
+      <c r="C96" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -2522,11 +2531,11 @@
       <c r="B97" s="10">
         <v>1300</v>
       </c>
-      <c r="C97" s="16" t="s">
-        <v>14</v>
+      <c r="C97" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E97" s="1"/>
     </row>
@@ -2537,26 +2546,26 @@
       <c r="B98" s="10">
         <v>1300</v>
       </c>
-      <c r="C98" s="13" t="s">
-        <v>6</v>
+      <c r="C98" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B99" s="10">
-        <v>2500</v>
-      </c>
-      <c r="C99" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D99" s="6" t="s">
-        <v>103</v>
+        <v>1300</v>
+      </c>
+      <c r="C99" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="E99" s="1"/>
     </row>
@@ -2567,11 +2576,11 @@
       <c r="B100" s="10">
         <v>2500</v>
       </c>
-      <c r="C100" s="12" t="s">
-        <v>5</v>
+      <c r="C100" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E100" s="1"/>
     </row>
@@ -2582,26 +2591,26 @@
       <c r="B101" s="10">
         <v>2500</v>
       </c>
-      <c r="C101" s="14" t="s">
-        <v>8</v>
+      <c r="C101" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B102" s="10">
-        <v>6000</v>
-      </c>
-      <c r="C102" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>106</v>
+        <v>2500</v>
+      </c>
+      <c r="C102" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="E102" s="1"/>
     </row>
@@ -2612,11 +2621,11 @@
       <c r="B103" s="10">
         <v>6000</v>
       </c>
-      <c r="C103" s="14" t="s">
-        <v>8</v>
+      <c r="C103" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E103" s="1"/>
     </row>
@@ -2627,26 +2636,26 @@
       <c r="B104" s="10">
         <v>6000</v>
       </c>
-      <c r="C104" s="16" t="s">
+      <c r="C104" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E104" s="1"/>
+    </row>
+    <row r="105" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B105" s="10">
+        <v>6000</v>
+      </c>
+      <c r="C105" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D105" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="E104" s="1"/>
-    </row>
-    <row r="105" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="B105" s="10">
-        <v>5400</v>
-      </c>
-      <c r="C105" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="E105" s="1"/>
     </row>
@@ -2657,11 +2666,11 @@
       <c r="B106" s="10">
         <v>5400</v>
       </c>
-      <c r="C106" s="12" t="s">
-        <v>5</v>
+      <c r="C106" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E106" s="1"/>
     </row>
@@ -2672,26 +2681,26 @@
       <c r="B107" s="10">
         <v>5400</v>
       </c>
-      <c r="C107" s="16" t="s">
+      <c r="C107" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E107" s="1"/>
+    </row>
+    <row r="108" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B108" s="10">
+        <v>5400</v>
+      </c>
+      <c r="C108" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="D108" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="E107" s="1"/>
-    </row>
-    <row r="108" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B108" s="10">
-        <v>1000</v>
-      </c>
-      <c r="C108" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="E108" s="1"/>
     </row>
@@ -2702,11 +2711,11 @@
       <c r="B109" s="10">
         <v>1000</v>
       </c>
-      <c r="C109" s="16" t="s">
-        <v>14</v>
+      <c r="C109" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>109</v>
+        <v>154</v>
       </c>
       <c r="E109" s="1"/>
     </row>
@@ -2717,26 +2726,26 @@
       <c r="B110" s="10">
         <v>1000</v>
       </c>
-      <c r="C110" s="13" t="s">
-        <v>6</v>
+      <c r="C110" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E110" s="1"/>
     </row>
     <row r="111" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B111" s="10">
-        <v>1900</v>
-      </c>
-      <c r="C111" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>111</v>
+        <v>1000</v>
+      </c>
+      <c r="C111" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E111" s="1"/>
     </row>
@@ -2747,11 +2756,11 @@
       <c r="B112" s="10">
         <v>1900</v>
       </c>
-      <c r="C112" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>112</v>
+      <c r="C112" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="E112" s="1"/>
     </row>
@@ -2762,11 +2771,11 @@
       <c r="B113" s="10">
         <v>1900</v>
       </c>
-      <c r="C113" s="15" t="s">
-        <v>9</v>
+      <c r="C113" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E113" s="1"/>
     </row>
@@ -2777,11 +2786,11 @@
       <c r="B114" s="10">
         <v>1900</v>
       </c>
-      <c r="C114" s="16" t="s">
-        <v>14</v>
+      <c r="C114" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E114" s="1"/>
     </row>
@@ -2792,26 +2801,26 @@
       <c r="B115" s="10">
         <v>1900</v>
       </c>
-      <c r="C115" s="13" t="s">
+      <c r="C115" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E115" s="1"/>
+    </row>
+    <row r="116" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B116" s="10">
+        <v>1900</v>
+      </c>
+      <c r="C116" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="D116" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="E115" s="1"/>
-    </row>
-    <row r="116" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B116" s="10">
-        <v>7000</v>
-      </c>
-      <c r="C116" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="E116" s="1"/>
     </row>
@@ -2822,11 +2831,11 @@
       <c r="B117" s="10">
         <v>7000</v>
       </c>
-      <c r="C117" s="14" t="s">
-        <v>8</v>
+      <c r="C117" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E117" s="1"/>
     </row>
@@ -2837,26 +2846,26 @@
       <c r="B118" s="10">
         <v>7000</v>
       </c>
-      <c r="C118" s="15" t="s">
+      <c r="C118" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E118" s="1"/>
+    </row>
+    <row r="119" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B119" s="10">
+        <v>7000</v>
+      </c>
+      <c r="C119" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D119" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="E118" s="1"/>
-    </row>
-    <row r="119" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B119" s="10">
-        <v>4000</v>
-      </c>
-      <c r="C119" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="E119" s="1"/>
     </row>
@@ -2867,11 +2876,11 @@
       <c r="B120" s="10">
         <v>4000</v>
       </c>
-      <c r="C120" s="15" t="s">
-        <v>9</v>
+      <c r="C120" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E120" s="1"/>
     </row>
@@ -2882,26 +2891,26 @@
       <c r="B121" s="10">
         <v>4000</v>
       </c>
-      <c r="C121" s="16" t="s">
-        <v>14</v>
+      <c r="C121" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B122" s="10">
-        <v>6500</v>
-      </c>
-      <c r="C122" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D122" s="4" t="s">
-        <v>103</v>
+        <v>4000</v>
+      </c>
+      <c r="C122" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="E122" s="1"/>
     </row>
@@ -2912,11 +2921,11 @@
       <c r="B123" s="10">
         <v>6500</v>
       </c>
-      <c r="C123" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D123" s="7" t="s">
-        <v>119</v>
+      <c r="C123" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="E123" s="1"/>
     </row>
@@ -2927,11 +2936,11 @@
       <c r="B124" s="10">
         <v>6500</v>
       </c>
-      <c r="C124" s="14" t="s">
-        <v>8</v>
+      <c r="C124" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E124" s="1"/>
     </row>
@@ -2942,11 +2951,11 @@
       <c r="B125" s="10">
         <v>6500</v>
       </c>
-      <c r="C125" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>121</v>
+      <c r="C125" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="E125" s="1"/>
     </row>
@@ -2957,11 +2966,11 @@
       <c r="B126" s="10">
         <v>6500</v>
       </c>
-      <c r="C126" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D126" s="7" t="s">
-        <v>122</v>
+      <c r="C126" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="E126" s="1"/>
     </row>
@@ -2972,34 +2981,35 @@
       <c r="B127" s="10">
         <v>6500</v>
       </c>
-      <c r="C127" s="13" t="s">
-        <v>6</v>
+      <c r="C127" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D127" s="7" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="E127" s="1"/>
     </row>
     <row r="128" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="9" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="B128" s="10">
-        <v>5800</v>
-      </c>
-      <c r="C128" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D128" s="10">
-        <v>99999</v>
-      </c>
+        <v>6500</v>
+      </c>
+      <c r="C128" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E128" s="1"/>
     </row>
     <row r="129" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="9" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="B129" s="10">
-        <v>4400</v>
+        <v>5800</v>
       </c>
       <c r="C129" s="11" t="s">
         <v>12</v>
@@ -3010,10 +3020,10 @@
     </row>
     <row r="130" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="9" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B130" s="10">
-        <v>5900</v>
+        <v>4400</v>
       </c>
       <c r="C130" s="11" t="s">
         <v>12</v>
@@ -3022,23 +3032,53 @@
         <v>99999</v>
       </c>
     </row>
+    <row r="131" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B131" s="10">
+        <v>5900</v>
+      </c>
+      <c r="C131" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D131" s="10">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B132" s="20">
+        <v>7200</v>
+      </c>
+      <c r="C132" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D132" s="10">
+        <v>99999</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D24" r:id="rId1" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{76D85841-0E92-4011-A17D-A4C4F39B78A0}"/>
-    <hyperlink ref="D25" r:id="rId2" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{C9A79CA9-B167-443A-AB21-1EA20451173E}"/>
-    <hyperlink ref="D26" r:id="rId3" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{6D2A01E7-99B9-4DCA-8F10-0193BA4220F1}"/>
-    <hyperlink ref="D43" r:id="rId4" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{22C1094A-0EAE-42D9-B543-021DD6A2C36F}"/>
-    <hyperlink ref="D44" r:id="rId5" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{7E462E08-4B0C-476D-AA36-E11FA80272FA}"/>
-    <hyperlink ref="D45" r:id="rId6" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{13B4A8AE-B629-42F9-B867-9E81A7263C7A}"/>
-    <hyperlink ref="D91" r:id="rId7" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{C28604FE-26D1-453D-8E55-BF4C270F28C4}"/>
-    <hyperlink ref="D92" r:id="rId8" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{E9917C5C-D5F0-4AD9-A2ED-472C92E6011C}"/>
-    <hyperlink ref="D111" r:id="rId9" display="http://puchakraborty.cm/" xr:uid="{02AFB277-C913-480D-BB5B-879E6BB17D14}"/>
-    <hyperlink ref="D21" r:id="rId10" xr:uid="{FCE7A3BF-4446-4E9F-83A0-11A360F0A079}"/>
-    <hyperlink ref="A72" r:id="rId11" tooltip="Optum Care Network - Idaho" display="javascript:void(0);" xr:uid="{90E131F6-422B-407C-B173-D7B05E9A01F6}"/>
-    <hyperlink ref="A80" r:id="rId12" tooltip="Optum Kansas City" display="javascript:void(0);" xr:uid="{ED7C1925-38C1-4B1C-BD55-4AC2E2B634E2}"/>
+    <hyperlink ref="D25" r:id="rId1" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{76D85841-0E92-4011-A17D-A4C4F39B78A0}"/>
+    <hyperlink ref="D26" r:id="rId2" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{C9A79CA9-B167-443A-AB21-1EA20451173E}"/>
+    <hyperlink ref="D27" r:id="rId3" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{6D2A01E7-99B9-4DCA-8F10-0193BA4220F1}"/>
+    <hyperlink ref="D44" r:id="rId4" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{22C1094A-0EAE-42D9-B543-021DD6A2C36F}"/>
+    <hyperlink ref="D45" r:id="rId5" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{7E462E08-4B0C-476D-AA36-E11FA80272FA}"/>
+    <hyperlink ref="D46" r:id="rId6" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{13B4A8AE-B629-42F9-B867-9E81A7263C7A}"/>
+    <hyperlink ref="D92" r:id="rId7" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{C28604FE-26D1-453D-8E55-BF4C270F28C4}"/>
+    <hyperlink ref="D93" r:id="rId8" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{E9917C5C-D5F0-4AD9-A2ED-472C92E6011C}"/>
+    <hyperlink ref="D112" r:id="rId9" display="http://puchakraborty.cm/" xr:uid="{02AFB277-C913-480D-BB5B-879E6BB17D14}"/>
+    <hyperlink ref="D22" r:id="rId10" xr:uid="{FCE7A3BF-4446-4E9F-83A0-11A360F0A079}"/>
+    <hyperlink ref="A73" r:id="rId11" tooltip="Optum Care Network - Idaho" display="javascript:void(0);" xr:uid="{90E131F6-422B-407C-B173-D7B05E9A01F6}"/>
+    <hyperlink ref="A81" r:id="rId12" tooltip="Optum Kansas City" display="javascript:void(0);" xr:uid="{ED7C1925-38C1-4B1C-BD55-4AC2E2B634E2}"/>
+    <hyperlink ref="A5" r:id="rId13" tooltip="AllCare To You" display="javascript:void(0);" xr:uid="{1E06C2FB-CB65-473A-A7AB-61F4C0CFB7D8}"/>
+    <hyperlink ref="A132" r:id="rId14" tooltip="Western Health Advantage" display="javascript:void(0);" xr:uid="{B71BB41A-2606-4691-BAF5-FEA2AF25D99F}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Excel MSO Provider Delegate change
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\Desktop\RTVS Local Dist\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\PycharmProjects\Release-Team-Verification-Suite\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ACF4B7-9960-4464-BCA8-82EC08BDBD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8AD1A0-EA2C-42A0-915F-051002027DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6870" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>EXCL_CSmith</t>
   </si>
   <si>
-    <t>EXCL_SVielma</t>
-  </si>
-  <si>
     <t>EXCL_DKHAY</t>
   </si>
   <si>
@@ -498,6 +495,9 @@
     <t>Chinese Community Health Plan (CCHP)</t>
   </si>
   <si>
+    <t>alex.turchinsky@cchphealthplan.com</t>
+  </si>
+  <si>
     <t>Optum Care Colorado(NWST)</t>
   </si>
   <si>
@@ -540,7 +540,7 @@
     <t>Western Health Advantage</t>
   </si>
   <si>
-    <t>craig.reich@cchphealthplan.com</t>
+    <t>EXCL_AAgustin</t>
   </si>
 </sst>
 </file>
@@ -1072,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1083,7 +1083,7 @@
     <col min="4" max="4" width="34.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1100,7 +1100,7 @@
     </row>
     <row r="2" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" s="10">
         <v>99999</v>
@@ -1124,7 +1124,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -1139,7 +1139,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -1169,7 +1169,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -1184,11 +1184,11 @@
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -1214,7 +1214,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -1229,11 +1229,11 @@
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="13" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" s="10">
         <v>6800</v>
@@ -1289,7 +1289,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -1304,11 +1304,11 @@
         <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
@@ -1319,11 +1319,11 @@
         <v>9</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>13</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" s="1"/>
     </row>
@@ -1349,13 +1349,13 @@
         <v>6</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B19" s="10">
         <v>6700</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="22" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B22" s="10">
         <v>7500</v>
@@ -1409,7 +1409,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -1424,7 +1424,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E23" s="1"/>
     </row>
@@ -1439,11 +1439,11 @@
         <v>8</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>16</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>9</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E25" s="1"/>
     </row>
@@ -1469,7 +1469,7 @@
         <v>5</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E26" s="1"/>
     </row>
@@ -1484,7 +1484,7 @@
         <v>8</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E27" s="1"/>
     </row>
@@ -1499,7 +1499,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="1"/>
     </row>
@@ -1514,11 +1514,11 @@
         <v>8</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>18</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" s="1"/>
     </row>
@@ -1548,7 +1548,7 @@
       </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>19</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>14</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>21</v>
+        <v>171</v>
       </c>
       <c r="E32" s="1"/>
     </row>
@@ -1574,13 +1574,13 @@
         <v>6</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34" s="10">
         <v>1800</v>
@@ -1589,13 +1589,13 @@
         <v>5</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35" s="10">
         <v>1800</v>
@@ -1604,13 +1604,13 @@
         <v>8</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" s="10">
         <v>1800</v>
@@ -1619,13 +1619,13 @@
         <v>14</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" s="10">
         <v>1800</v>
@@ -1634,13 +1634,13 @@
         <v>6</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B38" s="10">
         <v>4300</v>
@@ -1649,13 +1649,13 @@
         <v>5</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B39" s="10">
         <v>3000</v>
@@ -1664,13 +1664,13 @@
         <v>5</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B40" s="10">
         <v>3000</v>
@@ -1679,13 +1679,13 @@
         <v>8</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B41" s="10">
         <v>3000</v>
@@ -1694,13 +1694,13 @@
         <v>9</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B42" s="10">
         <v>3000</v>
@@ -1709,13 +1709,13 @@
         <v>14</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B43" s="10">
         <v>3000</v>
@@ -1724,13 +1724,13 @@
         <v>6</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B44" s="10">
         <v>3500</v>
@@ -1739,13 +1739,13 @@
         <v>5</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B45" s="10">
         <v>3500</v>
@@ -1754,13 +1754,13 @@
         <v>8</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B46" s="10">
         <v>3500</v>
@@ -1769,13 +1769,13 @@
         <v>14</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B47" s="10">
         <v>200</v>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="48" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B48" s="10">
         <v>3600</v>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="49" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B49" s="10">
         <v>4600</v>
@@ -1814,13 +1814,13 @@
         <v>5</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B50" s="10">
         <v>4600</v>
@@ -1829,13 +1829,13 @@
         <v>8</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B51" s="10">
         <v>4600</v>
@@ -1844,13 +1844,13 @@
         <v>9</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B52" s="10">
         <v>4600</v>
@@ -1859,13 +1859,13 @@
         <v>6</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B53" s="10">
         <v>150</v>
@@ -1874,13 +1874,13 @@
         <v>5</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B54" s="10">
         <v>150</v>
@@ -1889,13 +1889,13 @@
         <v>8</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B55" s="10">
         <v>150</v>
@@ -1904,13 +1904,13 @@
         <v>9</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B56" s="10">
         <v>150</v>
@@ -1919,13 +1919,13 @@
         <v>14</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B57" s="10">
         <v>150</v>
@@ -1934,13 +1934,13 @@
         <v>6</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B58" s="10">
         <v>2700</v>
@@ -1953,9 +1953,9 @@
       </c>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B59" s="10">
         <v>2700</v>
@@ -1964,13 +1964,13 @@
         <v>14</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B60" s="10">
         <v>2000</v>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="61" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B61" s="10">
         <v>2100</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="62" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B62" s="10">
         <v>5600</v>
@@ -2009,13 +2009,13 @@
         <v>5</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B63" s="10">
         <v>5600</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="64" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B64" s="10">
         <v>2600</v>
@@ -2045,7 +2045,7 @@
     </row>
     <row r="65" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B65" s="10">
         <v>1100</v>
@@ -2054,13 +2054,13 @@
         <v>5</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B66" s="10">
         <v>1100</v>
@@ -2069,13 +2069,13 @@
         <v>8</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B67" s="10">
         <v>1100</v>
@@ -2084,13 +2084,13 @@
         <v>9</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B68" s="10">
         <v>1100</v>
@@ -2099,13 +2099,13 @@
         <v>6</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B69" s="10">
         <v>3300</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="70" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B70" s="10">
         <v>5100</v>
@@ -2135,7 +2135,7 @@
     </row>
     <row r="71" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B71" s="10">
         <v>7400</v>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="74" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B74" s="10">
         <v>6600</v>
@@ -2194,7 +2194,7 @@
     </row>
     <row r="75" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B75" s="10">
         <v>5200</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="76" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B76" s="10">
         <v>4800</v>
@@ -2224,7 +2224,7 @@
     </row>
     <row r="77" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B77" s="10">
         <v>5300</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="78" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B78" s="10">
         <v>4900</v>
@@ -2252,9 +2252,9 @@
       </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B79" s="10">
         <v>4100</v>
@@ -2269,7 +2269,7 @@
     </row>
     <row r="80" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B80" s="10">
         <v>5000</v>
@@ -2298,7 +2298,7 @@
     </row>
     <row r="82" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B82" s="10">
         <v>4500</v>
@@ -2313,7 +2313,7 @@
     </row>
     <row r="83" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B83" s="10">
         <v>3400</v>
@@ -2328,22 +2328,22 @@
     </row>
     <row r="84" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B84" s="10">
         <v>1200</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B85" s="10">
         <v>1200</v>
@@ -2358,7 +2358,7 @@
     </row>
     <row r="86" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B86" s="10">
         <v>1200</v>
@@ -2367,13 +2367,13 @@
         <v>8</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B87" s="10">
         <v>1200</v>
@@ -2382,13 +2382,13 @@
         <v>9</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B88" s="10">
         <v>3900</v>
@@ -2397,13 +2397,13 @@
         <v>5</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E88" s="1"/>
     </row>
-    <row r="89" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B89" s="10">
         <v>3900</v>
@@ -2412,13 +2412,13 @@
         <v>9</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E89" s="1"/>
     </row>
-    <row r="90" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B90" s="10">
         <v>3900</v>
@@ -2427,13 +2427,13 @@
         <v>14</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B91" s="10">
         <v>3900</v>
@@ -2442,13 +2442,13 @@
         <v>6</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E91" s="1"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B92" s="10">
         <v>3800</v>
@@ -2457,13 +2457,13 @@
         <v>5</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B93" s="10">
         <v>3800</v>
@@ -2472,13 +2472,13 @@
         <v>14</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B94" s="10">
         <v>3800</v>
@@ -2493,7 +2493,7 @@
     </row>
     <row r="95" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B95" s="10">
         <v>1300</v>
@@ -2502,13 +2502,13 @@
         <v>5</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B96" s="10">
         <v>1300</v>
@@ -2517,13 +2517,13 @@
         <v>8</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E96" s="1"/>
     </row>
-    <row r="97" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B97" s="10">
         <v>1300</v>
@@ -2532,13 +2532,13 @@
         <v>9</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E97" s="1"/>
     </row>
-    <row r="98" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B98" s="10">
         <v>1300</v>
@@ -2547,13 +2547,13 @@
         <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B99" s="10">
         <v>1300</v>
@@ -2562,28 +2562,28 @@
         <v>6</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B100" s="10">
         <v>2500</v>
       </c>
       <c r="C100" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B101" s="10">
         <v>2500</v>
@@ -2592,13 +2592,13 @@
         <v>5</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B102" s="10">
         <v>2500</v>
@@ -2607,13 +2607,13 @@
         <v>8</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B103" s="10">
         <v>6000</v>
@@ -2622,13 +2622,13 @@
         <v>5</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B104" s="10">
         <v>6000</v>
@@ -2637,13 +2637,13 @@
         <v>8</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E104" s="1"/>
     </row>
-    <row r="105" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B105" s="10">
         <v>6000</v>
@@ -2652,13 +2652,13 @@
         <v>14</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B106" s="10">
         <v>5400</v>
@@ -2667,13 +2667,13 @@
         <v>8</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B107" s="10">
         <v>5400</v>
@@ -2682,13 +2682,13 @@
         <v>5</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B108" s="10">
         <v>5400</v>
@@ -2697,13 +2697,13 @@
         <v>14</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B109" s="10">
         <v>1000</v>
@@ -2712,13 +2712,13 @@
         <v>5</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E109" s="1"/>
     </row>
-    <row r="110" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B110" s="10">
         <v>1000</v>
@@ -2727,13 +2727,13 @@
         <v>14</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E110" s="1"/>
     </row>
     <row r="111" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B111" s="10">
         <v>1000</v>
@@ -2742,13 +2742,13 @@
         <v>6</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E111" s="1"/>
     </row>
     <row r="112" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B112" s="10">
         <v>1900</v>
@@ -2757,13 +2757,13 @@
         <v>5</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E112" s="1"/>
     </row>
     <row r="113" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B113" s="10">
         <v>1900</v>
@@ -2772,13 +2772,13 @@
         <v>8</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E113" s="1"/>
     </row>
-    <row r="114" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B114" s="10">
         <v>1900</v>
@@ -2787,13 +2787,13 @@
         <v>9</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E114" s="1"/>
     </row>
-    <row r="115" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B115" s="10">
         <v>1900</v>
@@ -2802,13 +2802,13 @@
         <v>14</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E115" s="1"/>
     </row>
     <row r="116" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B116" s="10">
         <v>1900</v>
@@ -2817,13 +2817,13 @@
         <v>6</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E116" s="1"/>
     </row>
     <row r="117" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B117" s="10">
         <v>7000</v>
@@ -2838,7 +2838,7 @@
     </row>
     <row r="118" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B118" s="10">
         <v>7000</v>
@@ -2853,7 +2853,7 @@
     </row>
     <row r="119" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B119" s="10">
         <v>7000</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="120" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B120" s="10">
         <v>4000</v>
@@ -2877,13 +2877,13 @@
         <v>5</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E120" s="1"/>
     </row>
-    <row r="121" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B121" s="10">
         <v>4000</v>
@@ -2892,13 +2892,13 @@
         <v>9</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E121" s="1"/>
     </row>
-    <row r="122" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B122" s="10">
         <v>4000</v>
@@ -2907,28 +2907,28 @@
         <v>14</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B123" s="10">
         <v>6500</v>
       </c>
       <c r="C123" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B124" s="10">
         <v>6500</v>
@@ -2937,13 +2937,13 @@
         <v>5</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B125" s="10">
         <v>6500</v>
@@ -2952,13 +2952,13 @@
         <v>8</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E125" s="1"/>
     </row>
-    <row r="126" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B126" s="10">
         <v>6500</v>
@@ -2967,13 +2967,13 @@
         <v>9</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E126" s="1"/>
     </row>
-    <row r="127" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B127" s="10">
         <v>6500</v>
@@ -2982,13 +2982,13 @@
         <v>14</v>
       </c>
       <c r="D127" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E127" s="1"/>
     </row>
     <row r="128" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B128" s="10">
         <v>6500</v>
@@ -2997,13 +2997,13 @@
         <v>6</v>
       </c>
       <c r="D128" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E128" s="1"/>
     </row>
     <row r="129" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B129" s="10">
         <v>5800</v>
@@ -3017,7 +3017,7 @@
     </row>
     <row r="130" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B130" s="10">
         <v>4400</v>
@@ -3031,7 +3031,7 @@
     </row>
     <row r="131" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B131" s="10">
         <v>5900</v>
@@ -3068,13 +3068,15 @@
     <hyperlink ref="D92" r:id="rId7" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{C28604FE-26D1-453D-8E55-BF4C270F28C4}"/>
     <hyperlink ref="D93" r:id="rId8" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{E9917C5C-D5F0-4AD9-A2ED-472C92E6011C}"/>
     <hyperlink ref="D112" r:id="rId9" display="http://puchakraborty.cm/" xr:uid="{02AFB277-C913-480D-BB5B-879E6BB17D14}"/>
-    <hyperlink ref="A73" r:id="rId10" tooltip="Optum Care Network - Idaho" display="javascript:void(0);" xr:uid="{90E131F6-422B-407C-B173-D7B05E9A01F6}"/>
-    <hyperlink ref="A81" r:id="rId11" tooltip="Optum Kansas City" display="javascript:void(0);" xr:uid="{ED7C1925-38C1-4B1C-BD55-4AC2E2B634E2}"/>
-    <hyperlink ref="A5" r:id="rId12" tooltip="AllCare To You" display="javascript:void(0);" xr:uid="{1E06C2FB-CB65-473A-A7AB-61F4C0CFB7D8}"/>
-    <hyperlink ref="A132" r:id="rId13" tooltip="Western Health Advantage" display="javascript:void(0);" xr:uid="{B71BB41A-2606-4691-BAF5-FEA2AF25D99F}"/>
+    <hyperlink ref="D22" r:id="rId10" xr:uid="{FCE7A3BF-4446-4E9F-83A0-11A360F0A079}"/>
+    <hyperlink ref="A73" r:id="rId11" tooltip="Optum Care Network - Idaho" display="javascript:void(0);" xr:uid="{90E131F6-422B-407C-B173-D7B05E9A01F6}"/>
+    <hyperlink ref="A81" r:id="rId12" tooltip="Optum Kansas City" display="javascript:void(0);" xr:uid="{ED7C1925-38C1-4B1C-BD55-4AC2E2B634E2}"/>
+    <hyperlink ref="A5" r:id="rId13" tooltip="AllCare To You" display="javascript:void(0);" xr:uid="{1E06C2FB-CB65-473A-A7AB-61F4C0CFB7D8}"/>
+    <hyperlink ref="A132" r:id="rId14" tooltip="Western Health Advantage" display="javascript:void(0);" xr:uid="{B71BB41A-2606-4691-BAF5-FEA2AF25D99F}"/>
+    <hyperlink ref="D32" r:id="rId15" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTIwMCZvcmdJZD0yMDAmcXVhcnRlcj0yMDIzLTEyLTMx&amp;person_id=47287683&amp;forPersonCustId=2900" xr:uid="{80C65B54-C905-474E-9487-7FDC76BA01D8}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId16"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Imperial Health CU user
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\Desktop\RTVS Local Dist\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFE8249-8C20-4D68-8114-15291E393D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9EE732-B1C2-4A5E-AFD6-8CE91DFCB6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="187">
   <si>
     <t>Customer Name</t>
   </si>
@@ -583,6 +583,9 @@
   </si>
   <si>
     <t>craig.reich@cchphealthplan.com</t>
+  </si>
+  <si>
+    <t>imphp_cloe.butial</t>
   </si>
 </sst>
 </file>
@@ -733,7 +736,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -789,6 +792,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1106,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2996,11 +3000,11 @@
       <c r="B53" s="7">
         <v>2350</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" s="7">
-        <v>99999</v>
+      <c r="C53" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>186</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -6313,9 +6317,10 @@
     <hyperlink ref="D51" r:id="rId8" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{0109AA83-5E18-4786-B03E-9777A15B64CF}"/>
     <hyperlink ref="D123" r:id="rId9" display="http://puchakraborty.cm/" xr:uid="{307A7FC4-2066-4A12-B303-9F9FF490B86E}"/>
     <hyperlink ref="D24" r:id="rId10" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmZG9jdG9yc1BlcnNvbklkPTk2MjI1NDQmZG9jdG9yX3VpZD05NjAyNDU1JnBheWVySWQ9MTUwMCZxdWFydGVyPTIwMjMtMTItMzEmaG9tZT1ZWEJ3WDJsa1BYSmxaMmx6ZEhKcFpYTW1ZM1Z6ZEVsa1BURTFNREFtY0dGNVpYSkpaRDB4TlRBd0ptOXlaMGxrUFRFMU1EQW1kbWR3U1dROU1UVXdNQ1oyY0Vsa1BURTFNREE&amp;person_id=49706900&amp;forPersonCustId=7500" xr:uid="{CC18F32E-C09E-4CA5-97D0-878614ABE42D}"/>
+    <hyperlink ref="D53" r:id="rId11" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTMwMDAmb3JnSWQ9MzAwMCZ2Z3BJZD0zMDAwJnZwSWQ9MzAwMA&amp;person_id=59064038&amp;forPersonCustId=2350" xr:uid="{8894B148-5BC9-45EF-9724-E71F502C83DF}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
chrome 122 and username sync
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\Desktop\RTVS Local Dist\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542D777A-0988-44B8-AC23-00ED158BB03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BD3808-EA5B-42A2-91D9-C853FE8593EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="206">
   <si>
     <t>Customer Name</t>
   </si>
@@ -228,9 +228,6 @@
     <t>dhmf_abajwa</t>
   </si>
   <si>
-    <t>ProviderBMG</t>
-  </si>
-  <si>
     <t>Jhall_FCA</t>
   </si>
   <si>
@@ -282,9 +279,6 @@
     <t>PIH_aacha</t>
   </si>
   <si>
-    <t>Pih_dchinchilla</t>
-  </si>
-  <si>
     <t>ppmsi_aaschim</t>
   </si>
   <si>
@@ -339,18 +333,9 @@
     <t>puchakraborty.cm.sequoia</t>
   </si>
   <si>
-    <t>SIH_AHuang</t>
-  </si>
-  <si>
     <t>SIH_LWilbourn</t>
   </si>
   <si>
-    <t>sequoia_office_admin</t>
-  </si>
-  <si>
-    <t>SIH_BJohnson</t>
-  </si>
-  <si>
     <t>sharp_lagbr</t>
   </si>
   <si>
@@ -402,21 +387,9 @@
     <t>Sharp Community Medical Group</t>
   </si>
   <si>
-    <t>Allcare_abueno</t>
-  </si>
-  <si>
     <t>Allcare_fbandookwala</t>
   </si>
   <si>
-    <t>altamed_abarsegyan</t>
-  </si>
-  <si>
-    <t>altamed_amacwan</t>
-  </si>
-  <si>
-    <t>abanerjee</t>
-  </si>
-  <si>
     <t>altamed_kprice</t>
   </si>
   <si>
@@ -435,18 +408,12 @@
     <t>GNP_Bwoods</t>
   </si>
   <si>
-    <t>MCMF_Jmollineda</t>
-  </si>
-  <si>
     <t>dbouyear_pracDel</t>
   </si>
   <si>
     <t>aomalley</t>
   </si>
   <si>
-    <t>SNguyen7</t>
-  </si>
-  <si>
     <t>MRTG_JMcIsaac</t>
   </si>
   <si>
@@ -601,13 +568,88 @@
   </si>
   <si>
     <t>wha_jbaillie</t>
+  </si>
+  <si>
+    <t>Allcare_abaca</t>
+  </si>
+  <si>
+    <t>AltaMed_AlUtria</t>
+  </si>
+  <si>
+    <t>altamed_aavila</t>
+  </si>
+  <si>
+    <t>AltaMed_Abigail</t>
+  </si>
+  <si>
+    <t>Bjohnson</t>
+  </si>
+  <si>
+    <t>Ofiice Admin</t>
+  </si>
+  <si>
+    <t>Adesbaillets</t>
+  </si>
+  <si>
+    <t>epic_cgibson</t>
+  </si>
+  <si>
+    <t>LaSalle Medical Associates</t>
+  </si>
+  <si>
+    <t>LSMA_SToubal</t>
+  </si>
+  <si>
+    <t>LSMA_Eaquino</t>
+  </si>
+  <si>
+    <t>adriene.przekop</t>
+  </si>
+  <si>
+    <t>EMG_sarnold</t>
+  </si>
+  <si>
+    <t>MCSHP_AdkinsDwivedi</t>
+  </si>
+  <si>
+    <t>mcshp_aamaya</t>
+  </si>
+  <si>
+    <t>SPatel4</t>
+  </si>
+  <si>
+    <t>PIH_aaldrete</t>
+  </si>
+  <si>
+    <t>SIH_TGleason</t>
+  </si>
+  <si>
+    <t>SIH_CHer</t>
+  </si>
+  <si>
+    <t>SIH_APatel</t>
+  </si>
+  <si>
+    <t>TMIPA_cteng</t>
+  </si>
+  <si>
+    <t>TMIPA_aip</t>
+  </si>
+  <si>
+    <t>Office Admin Practice and Provider Delegate</t>
+  </si>
+  <si>
+    <t>TMIPA_Apartovi</t>
+  </si>
+  <si>
+    <t>TMIPA_ctsuneishi2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -634,6 +676,11 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -809,7 +856,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -847,9 +894,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -869,6 +913,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1186,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z149"/>
+  <dimension ref="A1:Z158"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1237,7 +1287,7 @@
     </row>
     <row r="2" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B2" s="6">
         <v>99999</v>
@@ -1281,8 +1331,8 @@
       <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>125</v>
+      <c r="D3" s="20" t="s">
+        <v>181</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1318,7 +1368,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1345,7 +1395,7 @@
     </row>
     <row r="5" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B5" s="6">
         <v>1750</v>
@@ -1381,7 +1431,7 @@
     </row>
     <row r="6" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B6" s="6">
         <v>2750</v>
@@ -1426,7 +1476,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>127</v>
+        <v>182</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1461,8 +1511,8 @@
       <c r="C8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>128</v>
+      <c r="D8" s="12" t="s">
+        <v>183</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1494,11 +1544,11 @@
       <c r="B9" s="6">
         <v>1500</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>129</v>
+        <v>184</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1534,7 +1584,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1561,7 +1611,7 @@
     </row>
     <row r="11" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B11" s="6">
         <v>2650</v>
@@ -1642,7 +1692,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1674,7 +1724,7 @@
       <c r="B14" s="6">
         <v>3700</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="8" t="s">
@@ -1705,7 +1755,7 @@
     </row>
     <row r="15" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B15" s="6">
         <v>2600</v>
@@ -1777,7 +1827,7 @@
     </row>
     <row r="17" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B17" s="6">
         <v>6800</v>
@@ -1858,7 +1908,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1890,7 +1940,7 @@
       <c r="B20" s="6">
         <v>1600</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="8" t="s">
@@ -1926,7 +1976,7 @@
       <c r="B21" s="6">
         <v>1600</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="8" t="s">
@@ -1993,7 +2043,7 @@
     </row>
     <row r="23" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B23" s="6">
         <v>6700</v>
@@ -2029,7 +2079,7 @@
     </row>
     <row r="24" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B24" s="6">
         <v>7100</v>
@@ -2038,7 +2088,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -2063,18 +2113,18 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>15</v>
+        <v>135</v>
       </c>
       <c r="B25" s="6">
-        <v>4700</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="8">
-        <v>99999</v>
+        <v>7100</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>185</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="2"/>
@@ -2099,18 +2149,18 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="B26" s="6">
-        <v>7500</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>5</v>
+        <v>7100</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -2137,16 +2187,16 @@
     </row>
     <row r="27" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>175</v>
+        <v>15</v>
       </c>
       <c r="B27" s="6">
-        <v>7500</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>181</v>
+        <v>4700</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="8">
+        <v>99999</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2171,18 +2221,18 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>16</v>
+        <v>164</v>
       </c>
       <c r="B28" s="6">
-        <v>3200</v>
+        <v>7500</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>62</v>
+        <v>165</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -2207,18 +2257,18 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>16</v>
+        <v>164</v>
       </c>
       <c r="B29" s="6">
-        <v>3200</v>
+        <v>7500</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>63</v>
+        <v>170</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2250,11 +2300,11 @@
       <c r="B30" s="6">
         <v>3200</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>64</v>
+      <c r="C30" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -2281,16 +2331,16 @@
     </row>
     <row r="31" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>153</v>
+        <v>16</v>
       </c>
       <c r="B31" s="6">
-        <v>2050</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="8">
-        <v>99999</v>
+        <v>3200</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -2317,16 +2367,16 @@
     </row>
     <row r="32" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" s="6">
-        <v>3100</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>65</v>
+        <v>3200</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>64</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2353,16 +2403,16 @@
     </row>
     <row r="33" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>17</v>
+        <v>142</v>
       </c>
       <c r="B33" s="6">
-        <v>3100</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>66</v>
+        <v>2050</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="8">
+        <v>99999</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2394,11 +2444,11 @@
       <c r="B34" s="6">
         <v>3100</v>
       </c>
-      <c r="C34" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>154</v>
+      <c r="C34" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>65</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2425,16 +2475,16 @@
     </row>
     <row r="35" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" s="6">
-        <v>1700</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>182</v>
+        <v>3100</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2461,16 +2511,16 @@
     </row>
     <row r="36" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" s="6">
-        <v>1700</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>183</v>
+        <v>3100</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2502,11 +2552,11 @@
       <c r="B37" s="6">
         <v>1700</v>
       </c>
-      <c r="C37" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>67</v>
+      <c r="C37" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>171</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2533,16 +2583,16 @@
     </row>
     <row r="38" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" s="6">
-        <v>2900</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>20</v>
+        <v>1700</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>172</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2569,16 +2619,16 @@
     </row>
     <row r="39" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" s="6">
-        <v>2900</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>155</v>
+        <v>1700</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>188</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2610,11 +2660,11 @@
       <c r="B40" s="6">
         <v>2900</v>
       </c>
-      <c r="C40" s="15" t="s">
-        <v>14</v>
+      <c r="C40" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>184</v>
+        <v>20</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2646,11 +2696,11 @@
       <c r="B41" s="6">
         <v>2900</v>
       </c>
-      <c r="C41" s="10" t="s">
-        <v>6</v>
+      <c r="C41" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>21</v>
+        <v>144</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2677,16 +2727,16 @@
     </row>
     <row r="42" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B42" s="6">
-        <v>1800</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>5</v>
+        <v>2900</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>68</v>
+        <v>173</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2713,16 +2763,16 @@
     </row>
     <row r="43" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B43" s="6">
-        <v>1800</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>8</v>
+        <v>2900</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2754,11 +2804,11 @@
       <c r="B44" s="6">
         <v>1800</v>
       </c>
-      <c r="C44" s="15" t="s">
-        <v>14</v>
+      <c r="C44" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2790,11 +2840,11 @@
       <c r="B45" s="6">
         <v>1800</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>6</v>
+      <c r="C45" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2821,16 +2871,16 @@
     </row>
     <row r="46" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B46" s="6">
-        <v>4300</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>185</v>
+        <v>1800</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2857,16 +2907,16 @@
     </row>
     <row r="47" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B47" s="6">
-        <v>3000</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>72</v>
+        <v>1800</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2893,16 +2943,16 @@
     </row>
     <row r="48" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="6">
-        <v>3000</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>131</v>
+        <v>4300</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>174</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2934,11 +2984,11 @@
       <c r="B49" s="6">
         <v>3000</v>
       </c>
-      <c r="C49" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>132</v>
+      <c r="C49" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2970,11 +3020,11 @@
       <c r="B50" s="6">
         <v>3000</v>
       </c>
-      <c r="C50" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>133</v>
+      <c r="C50" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -3006,11 +3056,11 @@
       <c r="B51" s="6">
         <v>3000</v>
       </c>
-      <c r="C51" s="10" t="s">
-        <v>6</v>
+      <c r="C51" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>186</v>
+        <v>123</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -3037,16 +3087,16 @@
     </row>
     <row r="52" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B52" s="6">
-        <v>3500</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="17" t="s">
-        <v>73</v>
+        <v>3000</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>124</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -3073,16 +3123,16 @@
     </row>
     <row r="53" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B53" s="6">
-        <v>3500</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>74</v>
+        <v>3000</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>175</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -3114,11 +3164,11 @@
       <c r="B54" s="6">
         <v>3500</v>
       </c>
-      <c r="C54" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>75</v>
+      <c r="C54" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>72</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -3145,16 +3195,16 @@
     </row>
     <row r="55" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B55" s="6">
-        <v>200</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D55" s="8">
-        <v>99999</v>
+        <v>3500</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>73</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -3181,16 +3231,16 @@
     </row>
     <row r="56" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>156</v>
+        <v>25</v>
       </c>
       <c r="B56" s="6">
-        <v>2350</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>187</v>
+        <v>3500</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -3217,10 +3267,10 @@
     </row>
     <row r="57" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B57" s="6">
-        <v>3600</v>
+        <v>200</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>12</v>
@@ -3253,16 +3303,16 @@
     </row>
     <row r="58" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>28</v>
+        <v>145</v>
       </c>
       <c r="B58" s="6">
-        <v>4600</v>
+        <v>2350</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="8" t="s">
-        <v>76</v>
+      <c r="D58" s="12" t="s">
+        <v>176</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -3289,16 +3339,16 @@
     </row>
     <row r="59" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B59" s="6">
-        <v>4600</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>77</v>
+        <v>3600</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="8">
+        <v>99999</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -3325,16 +3375,16 @@
     </row>
     <row r="60" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>28</v>
+        <v>189</v>
       </c>
       <c r="B60" s="6">
-        <v>4600</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>9</v>
+        <v>2650</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>78</v>
+        <v>190</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -3361,16 +3411,16 @@
     </row>
     <row r="61" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>28</v>
+        <v>189</v>
       </c>
       <c r="B61" s="6">
-        <v>4600</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>6</v>
+        <v>2650</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>134</v>
+        <v>191</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -3397,16 +3447,16 @@
     </row>
     <row r="62" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B62" s="6">
-        <v>150</v>
+        <v>4600</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -3433,16 +3483,16 @@
     </row>
     <row r="63" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B63" s="6">
-        <v>150</v>
+        <v>4600</v>
       </c>
       <c r="C63" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>136</v>
+        <v>76</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -3469,16 +3519,16 @@
     </row>
     <row r="64" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B64" s="6">
-        <v>150</v>
-      </c>
-      <c r="C64" s="14" t="s">
+        <v>4600</v>
+      </c>
+      <c r="C64" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -3505,16 +3555,16 @@
     </row>
     <row r="65" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B65" s="6">
-        <v>150</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>14</v>
+        <v>4600</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -3546,11 +3596,11 @@
       <c r="B66" s="6">
         <v>150</v>
       </c>
-      <c r="C66" s="10" t="s">
-        <v>6</v>
+      <c r="C66" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -3575,18 +3625,18 @@
       <c r="Y66" s="1"/>
       <c r="Z66" s="1"/>
     </row>
-    <row r="67" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>157</v>
+        <v>29</v>
       </c>
       <c r="B67" s="6">
-        <v>5700</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D67" s="8">
-        <v>99999</v>
+        <v>150</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>192</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -3613,16 +3663,16 @@
     </row>
     <row r="68" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B68" s="6">
-        <v>2700</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="18" t="s">
-        <v>177</v>
+        <v>150</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -3649,16 +3699,16 @@
     </row>
     <row r="69" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B69" s="6">
-        <v>2700</v>
-      </c>
-      <c r="C69" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C69" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -3685,16 +3735,16 @@
     </row>
     <row r="70" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>158</v>
+        <v>29</v>
       </c>
       <c r="B70" s="6">
-        <v>1950</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D70" s="8">
-        <v>99999</v>
+        <v>150</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>193</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -3719,18 +3769,18 @@
       <c r="Y70" s="1"/>
       <c r="Z70" s="1"/>
     </row>
-    <row r="71" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>31</v>
+        <v>146</v>
       </c>
       <c r="B71" s="6">
-        <v>2000</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" s="8">
-        <v>99999</v>
+        <v>5700</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>194</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -3755,18 +3805,18 @@
       <c r="Y71" s="1"/>
       <c r="Z71" s="1"/>
     </row>
-    <row r="72" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>32</v>
+        <v>146</v>
       </c>
       <c r="B72" s="6">
-        <v>2100</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D72" s="8">
-        <v>99999</v>
+        <v>5700</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -3793,16 +3843,16 @@
     </row>
     <row r="73" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
-        <v>115</v>
+        <v>30</v>
       </c>
       <c r="B73" s="6">
-        <v>5600</v>
+        <v>2700</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="8" t="s">
-        <v>116</v>
+      <c r="D73" s="17" t="s">
+        <v>166</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -3829,16 +3879,16 @@
     </row>
     <row r="74" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
-        <v>115</v>
+        <v>30</v>
       </c>
       <c r="B74" s="6">
-        <v>5600</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>8</v>
+        <v>2700</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -3865,16 +3915,16 @@
     </row>
     <row r="75" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
-        <v>33</v>
+        <v>147</v>
       </c>
       <c r="B75" s="6">
-        <v>1100</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>79</v>
+        <v>1950</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" s="8">
+        <v>99999</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -3901,16 +3951,16 @@
     </row>
     <row r="76" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B76" s="6">
-        <v>1100</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>80</v>
+        <v>2000</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="8">
+        <v>99999</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -3937,16 +3987,16 @@
     </row>
     <row r="77" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B77" s="6">
-        <v>1100</v>
-      </c>
-      <c r="C77" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>81</v>
+        <v>2100</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="8">
+        <v>99999</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -3973,16 +4023,16 @@
     </row>
     <row r="78" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="B78" s="6">
-        <v>1100</v>
-      </c>
-      <c r="C78" s="10" t="s">
-        <v>6</v>
+        <v>5600</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
@@ -4009,16 +4059,16 @@
     </row>
     <row r="79" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="B79" s="6">
-        <v>3300</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D79" s="8">
-        <v>99999</v>
+        <v>5600</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -4045,16 +4095,16 @@
     </row>
     <row r="80" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B80" s="6">
-        <v>4500</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D80" s="8">
-        <v>99999</v>
+        <v>1100</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -4081,16 +4131,16 @@
     </row>
     <row r="81" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B81" s="6">
-        <v>5100</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D81" s="8">
-        <v>99999</v>
+        <v>1100</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
@@ -4117,16 +4167,16 @@
     </row>
     <row r="82" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B82" s="6">
-        <v>7400</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D82" s="8">
-        <v>99999</v>
+        <v>1100</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -4151,18 +4201,18 @@
       <c r="Y82" s="1"/>
       <c r="Z82" s="1"/>
     </row>
-    <row r="83" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
-        <v>160</v>
+        <v>33</v>
       </c>
       <c r="B83" s="6">
-        <v>2800</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D83" s="8">
-        <v>99999</v>
+        <v>1100</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
@@ -4187,12 +4237,12 @@
       <c r="Y83" s="1"/>
       <c r="Z83" s="1"/>
     </row>
-    <row r="84" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>148</v>
+        <v>34</v>
       </c>
       <c r="B84" s="6">
-        <v>1550</v>
+        <v>3300</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>12</v>
@@ -4223,12 +4273,12 @@
       <c r="Y84" s="1"/>
       <c r="Z84" s="1"/>
     </row>
-    <row r="85" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
-        <v>121</v>
+        <v>42</v>
       </c>
       <c r="B85" s="6">
-        <v>6600</v>
+        <v>4500</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>12</v>
@@ -4259,12 +4309,12 @@
       <c r="Y85" s="1"/>
       <c r="Z85" s="1"/>
     </row>
-    <row r="86" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B86" s="6">
-        <v>5200</v>
+        <v>5100</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>12</v>
@@ -4295,12 +4345,12 @@
       <c r="Y86" s="1"/>
       <c r="Z86" s="1"/>
     </row>
-    <row r="87" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B87" s="6">
-        <v>4800</v>
+        <v>7400</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>12</v>
@@ -4333,10 +4383,10 @@
     </row>
     <row r="88" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="B88" s="6">
-        <v>5300</v>
+        <v>2800</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>12</v>
@@ -4369,10 +4419,10 @@
     </row>
     <row r="89" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
-        <v>39</v>
+        <v>137</v>
       </c>
       <c r="B89" s="6">
-        <v>4900</v>
+        <v>1550</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>12</v>
@@ -4403,12 +4453,12 @@
       <c r="Y89" s="1"/>
       <c r="Z89" s="1"/>
     </row>
-    <row r="90" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="B90" s="6">
-        <v>4100</v>
+        <v>6600</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>12</v>
@@ -4439,12 +4489,12 @@
       <c r="Y90" s="1"/>
       <c r="Z90" s="1"/>
     </row>
-    <row r="91" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B91" s="6">
-        <v>5000</v>
+        <v>5200</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>12</v>
@@ -4477,10 +4527,10 @@
     </row>
     <row r="92" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
-        <v>161</v>
+        <v>38</v>
       </c>
       <c r="B92" s="6">
-        <v>2450</v>
+        <v>4800</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>12</v>
@@ -4511,12 +4561,12 @@
       <c r="Y92" s="1"/>
       <c r="Z92" s="1"/>
     </row>
-    <row r="93" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="B93" s="6">
-        <v>1650</v>
+        <v>5300</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>12</v>
@@ -4547,12 +4597,12 @@
       <c r="Y93" s="1"/>
       <c r="Z93" s="1"/>
     </row>
-    <row r="94" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B94" s="6">
-        <v>3400</v>
+        <v>4900</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>12</v>
@@ -4585,16 +4635,16 @@
     </row>
     <row r="95" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B95" s="6">
-        <v>1200</v>
-      </c>
-      <c r="C95" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D95" s="8" t="s">
-        <v>83</v>
+        <v>4100</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D95" s="8">
+        <v>99999</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
@@ -4621,16 +4671,16 @@
     </row>
     <row r="96" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B96" s="6">
-        <v>1200</v>
-      </c>
-      <c r="C96" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>162</v>
+        <v>5000</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D96" s="8">
+        <v>99999</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
@@ -4655,18 +4705,18 @@
       <c r="Y96" s="1"/>
       <c r="Z96" s="1"/>
     </row>
-    <row r="97" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="B97" s="6">
-        <v>1200</v>
-      </c>
-      <c r="C97" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>84</v>
+        <v>2450</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D97" s="8">
+        <v>99999</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -4693,16 +4743,16 @@
     </row>
     <row r="98" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
       <c r="B98" s="6">
-        <v>1200</v>
-      </c>
-      <c r="C98" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>85</v>
+        <v>1650</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D98" s="8">
+        <v>99999</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -4729,16 +4779,16 @@
     </row>
     <row r="99" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B99" s="6">
-        <v>3900</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>86</v>
+        <v>3400</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D99" s="8">
+        <v>99999</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -4765,16 +4815,16 @@
     </row>
     <row r="100" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B100" s="6">
-        <v>3900</v>
-      </c>
-      <c r="C100" s="14" t="s">
-        <v>9</v>
+        <v>1200</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
@@ -4801,16 +4851,16 @@
     </row>
     <row r="101" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B101" s="6">
-        <v>3900</v>
-      </c>
-      <c r="C101" s="15" t="s">
-        <v>14</v>
+        <v>1200</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
@@ -4837,16 +4887,16 @@
     </row>
     <row r="102" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B102" s="6">
-        <v>3900</v>
-      </c>
-      <c r="C102" s="10" t="s">
-        <v>6</v>
+        <v>1200</v>
+      </c>
+      <c r="C102" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
@@ -4873,16 +4923,16 @@
     </row>
     <row r="103" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B103" s="6">
-        <v>3800</v>
-      </c>
-      <c r="C103" s="9" t="s">
-        <v>5</v>
+        <v>1200</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>90</v>
+        <v>196</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
@@ -4909,16 +4959,16 @@
     </row>
     <row r="104" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B104" s="6">
-        <v>3800</v>
-      </c>
-      <c r="C104" s="15" t="s">
-        <v>14</v>
+        <v>1200</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
@@ -4945,16 +4995,16 @@
     </row>
     <row r="105" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B105" s="6">
-        <v>3800</v>
-      </c>
-      <c r="C105" s="10" t="s">
-        <v>6</v>
+        <v>3900</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>164</v>
+        <v>84</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
@@ -4981,16 +5031,16 @@
     </row>
     <row r="106" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B106" s="6">
-        <v>1300</v>
-      </c>
-      <c r="C106" s="9" t="s">
-        <v>5</v>
+        <v>3900</v>
+      </c>
+      <c r="C106" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
@@ -5017,16 +5067,16 @@
     </row>
     <row r="107" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B107" s="6">
-        <v>1300</v>
-      </c>
-      <c r="C107" s="11" t="s">
-        <v>8</v>
+        <v>3900</v>
+      </c>
+      <c r="C107" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
@@ -5053,16 +5103,16 @@
     </row>
     <row r="108" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B108" s="6">
-        <v>1300</v>
-      </c>
-      <c r="C108" s="14" t="s">
-        <v>9</v>
+        <v>3900</v>
+      </c>
+      <c r="C108" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
@@ -5089,16 +5139,16 @@
     </row>
     <row r="109" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B109" s="6">
-        <v>1300</v>
-      </c>
-      <c r="C109" s="15" t="s">
-        <v>14</v>
+        <v>3800</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -5125,16 +5175,16 @@
     </row>
     <row r="110" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B110" s="6">
-        <v>1300</v>
-      </c>
-      <c r="C110" s="10" t="s">
-        <v>6</v>
+        <v>3800</v>
+      </c>
+      <c r="C110" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>95</v>
+        <v>152</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
@@ -5161,16 +5211,16 @@
     </row>
     <row r="111" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
-        <v>165</v>
+        <v>47</v>
       </c>
       <c r="B111" s="6">
-        <v>1850</v>
-      </c>
-      <c r="C111" s="9" t="s">
-        <v>5</v>
+        <v>3800</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
@@ -5197,16 +5247,16 @@
     </row>
     <row r="112" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
-        <v>165</v>
+        <v>48</v>
       </c>
       <c r="B112" s="6">
-        <v>1850</v>
-      </c>
-      <c r="C112" s="11" t="s">
-        <v>8</v>
+        <v>1300</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>188</v>
+        <v>89</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
@@ -5233,16 +5283,16 @@
     </row>
     <row r="113" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
-        <v>165</v>
+        <v>48</v>
       </c>
       <c r="B113" s="6">
-        <v>1850</v>
-      </c>
-      <c r="C113" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D113" s="20" t="s">
-        <v>189</v>
+        <v>1300</v>
+      </c>
+      <c r="C113" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
@@ -5269,16 +5319,16 @@
     </row>
     <row r="114" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B114" s="6">
-        <v>2500</v>
-      </c>
-      <c r="C114" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D114" s="20" t="s">
-        <v>96</v>
+        <v>1300</v>
+      </c>
+      <c r="C114" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
@@ -5305,16 +5355,16 @@
     </row>
     <row r="115" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B115" s="6">
-        <v>2500</v>
-      </c>
-      <c r="C115" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D115" s="20" t="s">
-        <v>97</v>
+        <v>1300</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
@@ -5341,16 +5391,16 @@
     </row>
     <row r="116" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B116" s="6">
-        <v>2500</v>
-      </c>
-      <c r="C116" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D116" s="20" t="s">
-        <v>98</v>
+        <v>1300</v>
+      </c>
+      <c r="C116" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
@@ -5377,16 +5427,16 @@
     </row>
     <row r="117" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="B117" s="6">
-        <v>6000</v>
+        <v>1850</v>
       </c>
       <c r="C117" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>99</v>
+        <v>155</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
@@ -5413,16 +5463,16 @@
     </row>
     <row r="118" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="B118" s="6">
-        <v>6000</v>
+        <v>1850</v>
       </c>
       <c r="C118" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -5449,16 +5499,16 @@
     </row>
     <row r="119" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="B119" s="6">
-        <v>6000</v>
-      </c>
-      <c r="C119" s="15" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C119" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D119" s="8" t="s">
-        <v>100</v>
+      <c r="D119" s="19" t="s">
+        <v>178</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
@@ -5485,16 +5535,16 @@
     </row>
     <row r="120" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B120" s="6">
-        <v>6000</v>
-      </c>
-      <c r="C120" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D120" s="8" t="s">
-        <v>168</v>
+        <v>2500</v>
+      </c>
+      <c r="C120" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D120" s="19" t="s">
+        <v>94</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
@@ -5519,18 +5569,18 @@
       <c r="Y120" s="1"/>
       <c r="Z120" s="1"/>
     </row>
-    <row r="121" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
-        <v>117</v>
+        <v>49</v>
       </c>
       <c r="B121" s="6">
-        <v>5400</v>
+        <v>2500</v>
       </c>
       <c r="C121" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D121" s="8" t="s">
-        <v>142</v>
+      <c r="D121" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
@@ -5555,18 +5605,18 @@
       <c r="Y121" s="1"/>
       <c r="Z121" s="1"/>
     </row>
-    <row r="122" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
-        <v>117</v>
+        <v>49</v>
       </c>
       <c r="B122" s="6">
-        <v>5400</v>
+        <v>2500</v>
       </c>
       <c r="C122" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D122" s="16" t="s">
-        <v>141</v>
+      <c r="D122" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
@@ -5591,18 +5641,18 @@
       <c r="Y122" s="1"/>
       <c r="Z122" s="1"/>
     </row>
-    <row r="123" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="B123" s="6">
-        <v>5400</v>
-      </c>
-      <c r="C123" s="15" t="s">
-        <v>14</v>
+        <v>6000</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
@@ -5627,18 +5677,18 @@
       <c r="Y123" s="1"/>
       <c r="Z123" s="1"/>
     </row>
-    <row r="124" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="B124" s="6">
-        <v>5400</v>
-      </c>
-      <c r="C124" s="14" t="s">
-        <v>9</v>
+        <v>6000</v>
+      </c>
+      <c r="C124" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
@@ -5665,16 +5715,16 @@
     </row>
     <row r="125" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B125" s="6">
-        <v>1000</v>
-      </c>
-      <c r="C125" s="9" t="s">
-        <v>5</v>
+        <v>6000</v>
+      </c>
+      <c r="C125" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -5701,16 +5751,16 @@
     </row>
     <row r="126" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B126" s="6">
-        <v>1000</v>
-      </c>
-      <c r="C126" s="15" t="s">
-        <v>14</v>
+        <v>6000</v>
+      </c>
+      <c r="C126" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>101</v>
+        <v>157</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
@@ -5735,18 +5785,18 @@
       <c r="Y126" s="1"/>
       <c r="Z126" s="1"/>
     </row>
-    <row r="127" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="B127" s="6">
-        <v>1000</v>
-      </c>
-      <c r="C127" s="10" t="s">
-        <v>6</v>
+        <v>5400</v>
+      </c>
+      <c r="C127" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
@@ -5771,18 +5821,18 @@
       <c r="Y127" s="1"/>
       <c r="Z127" s="1"/>
     </row>
-    <row r="128" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="B128" s="6">
-        <v>1900</v>
-      </c>
-      <c r="C128" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D128" s="8" t="s">
-        <v>103</v>
+        <v>5400</v>
+      </c>
+      <c r="C128" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D128" s="15" t="s">
+        <v>130</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
@@ -5807,18 +5857,18 @@
       <c r="Y128" s="1"/>
       <c r="Z128" s="1"/>
     </row>
-    <row r="129" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="B129" s="6">
-        <v>1900</v>
-      </c>
-      <c r="C129" s="11" t="s">
-        <v>8</v>
+        <v>5400</v>
+      </c>
+      <c r="C129" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
@@ -5843,18 +5893,18 @@
       <c r="Y129" s="1"/>
       <c r="Z129" s="1"/>
     </row>
-    <row r="130" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="5" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="B130" s="6">
-        <v>1900</v>
-      </c>
-      <c r="C130" s="14" t="s">
+        <v>5400</v>
+      </c>
+      <c r="C130" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -5881,16 +5931,16 @@
     </row>
     <row r="131" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B131" s="6">
-        <v>1900</v>
-      </c>
-      <c r="C131" s="15" t="s">
-        <v>14</v>
+        <v>1000</v>
+      </c>
+      <c r="C131" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
@@ -5917,16 +5967,16 @@
     </row>
     <row r="132" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B132" s="6">
-        <v>1900</v>
-      </c>
-      <c r="C132" s="10" t="s">
-        <v>6</v>
+        <v>1000</v>
+      </c>
+      <c r="C132" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
@@ -5951,18 +6001,18 @@
       <c r="Y132" s="1"/>
       <c r="Z132" s="1"/>
     </row>
-    <row r="133" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
-        <v>124</v>
+        <v>51</v>
       </c>
       <c r="B133" s="6">
-        <v>7000</v>
-      </c>
-      <c r="C133" s="9" t="s">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C133" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
@@ -5987,18 +6037,18 @@
       <c r="Y133" s="1"/>
       <c r="Z133" s="1"/>
     </row>
-    <row r="134" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
-        <v>124</v>
+        <v>52</v>
       </c>
       <c r="B134" s="6">
-        <v>7000</v>
-      </c>
-      <c r="C134" s="11" t="s">
-        <v>8</v>
+        <v>1900</v>
+      </c>
+      <c r="C134" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>171</v>
+        <v>101</v>
       </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
@@ -6023,18 +6073,18 @@
       <c r="Y134" s="1"/>
       <c r="Z134" s="1"/>
     </row>
-    <row r="135" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="5" t="s">
-        <v>124</v>
+        <v>52</v>
       </c>
       <c r="B135" s="6">
-        <v>7000</v>
-      </c>
-      <c r="C135" s="10" t="s">
-        <v>172</v>
+        <v>1900</v>
+      </c>
+      <c r="C135" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
@@ -6059,18 +6109,18 @@
       <c r="Y135" s="1"/>
       <c r="Z135" s="1"/>
     </row>
-    <row r="136" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="5" t="s">
-        <v>124</v>
+        <v>52</v>
       </c>
       <c r="B136" s="6">
-        <v>7000</v>
-      </c>
-      <c r="C136" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D136" s="8">
-        <v>99999</v>
+        <v>1900</v>
+      </c>
+      <c r="C136" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D136" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
@@ -6097,16 +6147,16 @@
     </row>
     <row r="137" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B137" s="6">
-        <v>4000</v>
-      </c>
-      <c r="C137" s="9" t="s">
-        <v>5</v>
+        <v>1900</v>
+      </c>
+      <c r="C137" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
@@ -6133,16 +6183,16 @@
     </row>
     <row r="138" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B138" s="6">
-        <v>4000</v>
-      </c>
-      <c r="C138" s="14" t="s">
-        <v>9</v>
+        <v>1900</v>
+      </c>
+      <c r="C138" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>108</v>
+        <v>200</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -6167,18 +6217,18 @@
       <c r="Y138" s="1"/>
       <c r="Z138" s="1"/>
     </row>
-    <row r="139" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="B139" s="6">
-        <v>4000</v>
-      </c>
-      <c r="C139" s="15" t="s">
-        <v>14</v>
+        <v>7000</v>
+      </c>
+      <c r="C139" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>109</v>
+        <v>159</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -6203,18 +6253,18 @@
       <c r="Y139" s="1"/>
       <c r="Z139" s="1"/>
     </row>
-    <row r="140" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="B140" s="6">
-        <v>6500</v>
-      </c>
-      <c r="C140" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D140" s="12" t="s">
-        <v>96</v>
+        <v>7000</v>
+      </c>
+      <c r="C140" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D140" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
@@ -6239,18 +6289,18 @@
       <c r="Y140" s="1"/>
       <c r="Z140" s="1"/>
     </row>
-    <row r="141" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="B141" s="6">
-        <v>6500</v>
-      </c>
-      <c r="C141" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D141" s="12" t="s">
-        <v>110</v>
+        <v>7000</v>
+      </c>
+      <c r="C141" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D141" s="8" t="s">
+        <v>162</v>
       </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
@@ -6275,18 +6325,18 @@
       <c r="Y141" s="1"/>
       <c r="Z141" s="1"/>
     </row>
-    <row r="142" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="5" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="B142" s="6">
-        <v>6500</v>
-      </c>
-      <c r="C142" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D142" s="12" t="s">
-        <v>111</v>
+        <v>7000</v>
+      </c>
+      <c r="C142" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D142" s="8">
+        <v>99999</v>
       </c>
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
@@ -6313,16 +6363,16 @@
     </row>
     <row r="143" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B143" s="6">
-        <v>6500</v>
-      </c>
-      <c r="C143" s="14" t="s">
-        <v>9</v>
+        <v>4000</v>
+      </c>
+      <c r="C143" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>112</v>
+        <v>163</v>
       </c>
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
@@ -6349,16 +6399,16 @@
     </row>
     <row r="144" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B144" s="6">
-        <v>6500</v>
-      </c>
-      <c r="C144" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D144" s="12" t="s">
-        <v>113</v>
+        <v>4000</v>
+      </c>
+      <c r="C144" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D144" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
@@ -6385,86 +6435,213 @@
     </row>
     <row r="145" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B145" s="6">
-        <v>6500</v>
-      </c>
-      <c r="C145" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D145" s="12" t="s">
-        <v>145</v>
+        <v>4000</v>
+      </c>
+      <c r="C145" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D145" s="8" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="5" t="s">
-        <v>119</v>
+        <v>54</v>
       </c>
       <c r="B146" s="6">
-        <v>5800</v>
-      </c>
-      <c r="C146" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D146" s="8">
-        <v>99999</v>
+        <v>6500</v>
+      </c>
+      <c r="C146" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B147" s="6">
-        <v>4400</v>
-      </c>
-      <c r="C147" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D147" s="8">
-        <v>99999</v>
+        <v>6500</v>
+      </c>
+      <c r="C147" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D147" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="5" t="s">
-        <v>120</v>
+        <v>54</v>
       </c>
       <c r="B148" s="6">
-        <v>5900</v>
-      </c>
-      <c r="C148" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D148" s="8">
-        <v>99999</v>
+        <v>6500</v>
+      </c>
+      <c r="C148" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D148" s="12" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="5" t="s">
-        <v>190</v>
+        <v>54</v>
       </c>
       <c r="B149" s="6">
+        <v>6500</v>
+      </c>
+      <c r="C149" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D149" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B150" s="6">
+        <v>6500</v>
+      </c>
+      <c r="C150" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D150" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A151" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B151" s="6">
+        <v>6500</v>
+      </c>
+      <c r="C151" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D151" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B152" s="6">
+        <v>5800</v>
+      </c>
+      <c r="C152" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D152" s="8">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B153" s="6">
+        <v>4400</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D153" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A154" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B154" s="6">
+        <v>4400</v>
+      </c>
+      <c r="C154" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D154" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A155" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B155" s="6">
+        <v>4400</v>
+      </c>
+      <c r="C155" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="D155" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B156" s="6">
+        <v>4400</v>
+      </c>
+      <c r="C156" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D156" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B157" s="6">
+        <v>5900</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D157" s="8">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A158" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B158" s="6">
         <v>7200</v>
       </c>
-      <c r="C149" s="9" t="s">
+      <c r="C158" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D149" s="12" t="s">
-        <v>191</v>
+      <c r="D158" s="12" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=9694765&amp;forPersonCustId=1500" xr:uid="{78F93C90-F5E6-4994-93A9-E773F683C047}"/>
-    <hyperlink ref="D30" r:id="rId2" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{CEE388AB-B290-47E1-B69C-7A4A6C2E0D07}"/>
-    <hyperlink ref="D32" r:id="rId3" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{7E82E94B-6C22-4B02-AFEA-1BC2F44C6318}"/>
-    <hyperlink ref="D33" r:id="rId4" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{CE9CE294-5CF6-42F5-986B-E47943E6D9FC}"/>
-    <hyperlink ref="D34" r:id="rId5" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37055482&amp;forPersonCustId=3100" xr:uid="{F089B761-0E96-48FA-B219-CD89A4EE2B80}"/>
-    <hyperlink ref="D52" r:id="rId6" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{94FD8B0D-B67A-4A93-A5BE-DB59E9061B14}"/>
-    <hyperlink ref="D54" r:id="rId7" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{34F049C9-E1C1-4811-8C33-82E26D8887DB}"/>
+    <hyperlink ref="D3" r:id="rId1" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTEwMDAmb3JnSWQ9MTAwMCZ2Z3BJZD0xMDAwJnZwSWQ9MTAwMCZ2ZzBJZD0xMDAw&amp;person_id=15873326&amp;forPersonCustId=2400" xr:uid="{3AA17D9F-0394-418F-8F81-415D653930D8}"/>
+    <hyperlink ref="D32" r:id="rId2" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{A1D049BC-03E8-42C1-966A-600E87E092A6}"/>
+    <hyperlink ref="D34" r:id="rId3" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{0BF47B9A-FA31-499C-A6E2-0564CAA08A51}"/>
+    <hyperlink ref="D35" r:id="rId4" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{7857E010-19F1-4D55-AAB5-C49682C31352}"/>
+    <hyperlink ref="D36" r:id="rId5" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37055482&amp;forPersonCustId=3100" xr:uid="{54B827EF-006E-4E2B-9D9F-755C0612BAEB}"/>
+    <hyperlink ref="D39" r:id="rId6" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTEwMDAmb3JnSWQ9MTAwMCZ2Z3BJZD0xMDAwJnZwSWQ9MTAwMCZ2ZzBJZD0xMDAw&amp;person_id=60458157&amp;forPersonCustId=1700" xr:uid="{24CDD955-5A01-4675-835E-7821BD74DDAA}"/>
+    <hyperlink ref="D54" r:id="rId7" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{E02C5E5F-1A97-4F6C-8E04-C7C1467BC8D9}"/>
+    <hyperlink ref="D56" r:id="rId8" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{36BA325E-B5F4-4546-ADDC-DEA213851D23}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Registry Overhaul fixes plus
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\PycharmProjects\Release-Team-Verification-Suite\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\Desktop\RTVS Local Dist\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C61B58D-463C-4AA2-B5C4-B05319DA4FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8FB58D-DC47-4186-A1D7-9904D0891852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -381,9 +381,6 @@
     <t>GNP_Bwoods</t>
   </si>
   <si>
-    <t>dbouyear_pracDel</t>
-  </si>
-  <si>
     <t>aomalley</t>
   </si>
   <si>
@@ -685,6 +682,9 @@
   </si>
   <si>
     <t>wha_sowens1</t>
+  </si>
+  <si>
+    <t>GNP_kim.holford</t>
   </si>
 </sst>
 </file>
@@ -1286,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H172" sqref="H172"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="3" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3" s="6">
         <v>4350</v>
@@ -1416,7 +1416,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1479,7 +1479,7 @@
     </row>
     <row r="6" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" s="6">
         <v>1750</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="7" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B7" s="6">
         <v>2750</v>
@@ -1560,7 +1560,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1596,7 +1596,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1632,7 +1632,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="13" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B13" s="6">
         <v>3750</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="14" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" s="6">
         <v>2600</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="16" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B16" s="6">
         <v>3250</v>
@@ -1920,7 +1920,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1956,7 +1956,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="23" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B23" s="6">
         <v>7100</v>
@@ -2100,7 +2100,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2127,7 +2127,7 @@
     </row>
     <row r="24" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B24" s="6">
         <v>7100</v>
@@ -2136,7 +2136,7 @@
         <v>8</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -2163,16 +2163,16 @@
     </row>
     <row r="25" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B25" s="6">
         <v>7100</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>169</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>170</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="2"/>
@@ -2235,7 +2235,7 @@
     </row>
     <row r="27" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B27" s="6">
         <v>7500</v>
@@ -2244,7 +2244,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2271,7 +2271,7 @@
     </row>
     <row r="28" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B28" s="6">
         <v>7500</v>
@@ -2280,7 +2280,7 @@
         <v>8</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -2415,7 +2415,7 @@
     </row>
     <row r="32" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B32" s="6">
         <v>2050</v>
@@ -2532,7 +2532,7 @@
         <v>14</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2568,7 +2568,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2604,7 +2604,7 @@
         <v>8</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2640,7 +2640,7 @@
         <v>9</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2712,7 +2712,7 @@
         <v>8</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2748,7 +2748,7 @@
         <v>14</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2964,7 +2964,7 @@
         <v>5</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -3144,7 +3144,7 @@
         <v>6</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -3180,7 +3180,7 @@
         <v>5</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -3315,7 +3315,7 @@
     </row>
     <row r="57" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B57" s="6">
         <v>4250</v>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="58" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B58" s="6">
         <v>2350</v>
@@ -3360,7 +3360,7 @@
         <v>5</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -3423,7 +3423,7 @@
     </row>
     <row r="60" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B60" s="6">
         <v>2250</v>
@@ -3459,7 +3459,7 @@
     </row>
     <row r="61" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B61" s="6">
         <v>2650</v>
@@ -3468,7 +3468,7 @@
         <v>5</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -3495,7 +3495,7 @@
     </row>
     <row r="62" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B62" s="6">
         <v>2650</v>
@@ -3504,7 +3504,7 @@
         <v>8</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -3720,7 +3720,7 @@
         <v>8</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -3755,8 +3755,8 @@
       <c r="C69" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D69" s="8" t="s">
-        <v>118</v>
+      <c r="D69" t="s">
+        <v>219</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -3792,7 +3792,7 @@
         <v>14</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -3828,7 +3828,7 @@
         <v>6</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -3855,7 +3855,7 @@
     </row>
     <row r="72" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B72" s="6">
         <v>5700</v>
@@ -3864,7 +3864,7 @@
         <v>5</v>
       </c>
       <c r="D72" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -3891,16 +3891,16 @@
     </row>
     <row r="73" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B73" s="6">
         <v>5700</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -3936,7 +3936,7 @@
         <v>5</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -3972,7 +3972,7 @@
         <v>14</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -3999,7 +3999,7 @@
     </row>
     <row r="76" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B76" s="6">
         <v>1950</v>
@@ -4152,7 +4152,7 @@
         <v>8</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -4179,7 +4179,7 @@
     </row>
     <row r="81" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B81" s="6">
         <v>3850</v>
@@ -4503,7 +4503,7 @@
     </row>
     <row r="90" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B90" s="6">
         <v>2800</v>
@@ -4539,7 +4539,7 @@
     </row>
     <row r="91" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B91" s="6">
         <v>1550</v>
@@ -4755,7 +4755,7 @@
     </row>
     <row r="97" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B97" s="6">
         <v>2950</v>
@@ -4827,7 +4827,7 @@
     </row>
     <row r="99" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B99" s="6">
         <v>3950</v>
@@ -4899,7 +4899,7 @@
     </row>
     <row r="101" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B101" s="6">
         <v>3550</v>
@@ -4935,7 +4935,7 @@
     </row>
     <row r="102" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B102" s="6">
         <v>3650</v>
@@ -4971,7 +4971,7 @@
     </row>
     <row r="103" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B103" s="6">
         <v>2450</v>
@@ -5007,7 +5007,7 @@
     </row>
     <row r="104" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B104" s="6">
         <v>3450</v>
@@ -5043,7 +5043,7 @@
     </row>
     <row r="105" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B105" s="6">
         <v>3350</v>
@@ -5079,7 +5079,7 @@
     </row>
     <row r="106" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B106" s="6">
         <v>1650</v>
@@ -5196,7 +5196,7 @@
         <v>5</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -5268,7 +5268,7 @@
         <v>6</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
@@ -5301,10 +5301,10 @@
         <v>1200</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
@@ -5475,7 +5475,7 @@
     </row>
     <row r="117" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B117" s="6">
         <v>2550</v>
@@ -5484,7 +5484,7 @@
         <v>5</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
@@ -5556,7 +5556,7 @@
         <v>14</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
@@ -5592,7 +5592,7 @@
         <v>6</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
@@ -5772,7 +5772,7 @@
         <v>6</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -5799,7 +5799,7 @@
     </row>
     <row r="126" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B126" s="6">
         <v>1850</v>
@@ -5808,7 +5808,7 @@
         <v>5</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
@@ -5835,7 +5835,7 @@
     </row>
     <row r="127" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B127" s="6">
         <v>1850</v>
@@ -5844,7 +5844,7 @@
         <v>8</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
@@ -5871,7 +5871,7 @@
     </row>
     <row r="128" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B128" s="6">
         <v>1850</v>
@@ -5880,7 +5880,7 @@
         <v>14</v>
       </c>
       <c r="D128" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
@@ -6060,7 +6060,7 @@
         <v>8</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
@@ -6132,7 +6132,7 @@
         <v>9</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
@@ -6168,7 +6168,7 @@
         <v>5</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
@@ -6204,7 +6204,7 @@
         <v>8</v>
       </c>
       <c r="D137" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
@@ -6240,7 +6240,7 @@
         <v>14</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -6276,7 +6276,7 @@
         <v>9</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -6303,7 +6303,7 @@
     </row>
     <row r="140" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B140" s="6">
         <v>3150</v>
@@ -6348,7 +6348,7 @@
         <v>5</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
@@ -6492,7 +6492,7 @@
         <v>8</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
@@ -6564,7 +6564,7 @@
         <v>14</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="148" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6578,7 +6578,7 @@
         <v>6</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="149" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6592,7 +6592,7 @@
         <v>5</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="150" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6606,7 +6606,7 @@
         <v>8</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="151" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6617,10 +6617,10 @@
         <v>7000</v>
       </c>
       <c r="C151" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D151" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="D151" s="8" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="152" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6648,7 +6648,7 @@
         <v>5</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="154" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6804,7 +6804,7 @@
         <v>6</v>
       </c>
       <c r="D161" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E161" s="1"/>
       <c r="F161" s="1"/>
@@ -6831,7 +6831,7 @@
     </row>
     <row r="162" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A162" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B162" s="6">
         <v>5800</v>
@@ -6845,7 +6845,7 @@
     </row>
     <row r="163" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A163" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B163" s="6">
         <v>4400</v>
@@ -6854,12 +6854,12 @@
         <v>5</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="164" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A164" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B164" s="6">
         <v>4400</v>
@@ -6868,26 +6868,26 @@
         <v>8</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="165" spans="1:26" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A165" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B165" s="6">
         <v>4400</v>
       </c>
       <c r="C165" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="D165" s="8" t="s">
         <v>210</v>
-      </c>
-      <c r="D165" s="8" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="166" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B166" s="6">
         <v>4400</v>
@@ -6896,12 +6896,12 @@
         <v>6</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="167" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A167" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B167" s="6">
         <v>5900</v>
@@ -6910,12 +6910,12 @@
         <v>5</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="168" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A168" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B168" s="6">
         <v>5900</v>
@@ -6924,12 +6924,12 @@
         <v>8</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="169" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A169" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B169" s="6">
         <v>5900</v>
@@ -6938,12 +6938,12 @@
         <v>14</v>
       </c>
       <c r="D169" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="170" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A170" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B170" s="6">
         <v>7200</v>
@@ -6952,12 +6952,12 @@
         <v>5</v>
       </c>
       <c r="D170" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="171" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B171" s="6">
         <v>7200</v>
@@ -6966,7 +6966,7 @@
         <v>8</v>
       </c>
       <c r="D171" s="23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support ticket env drop
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\Desktop\RTVS Local Dist\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8FB58D-DC47-4186-A1D7-9904D0891852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91ADE90F-AA15-4A9C-BDD7-10D546DD0A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1286,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Yet another support fix
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\Desktop\RTVS Local Dist\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA02061-C770-400A-B047-7B2296A8BB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F3C52E-FB2C-4ED3-A869-747CF5969269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="215">
   <si>
     <t>Customer Name</t>
   </si>
@@ -384,9 +384,6 @@
     <t>PROV_CA_AReyes</t>
   </si>
   <si>
-    <t>CHOC.llyGuerrero</t>
-  </si>
-  <si>
     <t>CHOC.aavellaneda</t>
   </si>
   <si>
@@ -597,12 +594,6 @@
     <t>Western Health Advantage</t>
   </si>
   <si>
-    <t>wha_jbaillie</t>
-  </si>
-  <si>
-    <t>wha_sowens1</t>
-  </si>
-  <si>
     <t>Aetna (CAPCI)</t>
   </si>
   <si>
@@ -676,6 +667,9 @@
   </si>
   <si>
     <t>Simulated Customer 2 (Deid)</t>
+  </si>
+  <si>
+    <t>Choc.GGomezBarajas</t>
   </si>
 </sst>
 </file>
@@ -1279,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z167"/>
+  <dimension ref="A1:Z166"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A152" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A161" sqref="A161"/>
+      <selection activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1366,7 +1360,7 @@
     </row>
     <row r="3" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" s="6">
         <v>4050</v>
@@ -1402,7 +1396,7 @@
     </row>
     <row r="4" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B4" s="6">
         <v>4350</v>
@@ -1447,7 +1441,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1546,7 +1540,7 @@
     </row>
     <row r="8" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8" s="6">
         <v>2750</v>
@@ -1582,7 +1576,7 @@
     </row>
     <row r="9" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B9" s="6">
         <v>1600</v>
@@ -1591,7 +1585,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1618,7 +1612,7 @@
     </row>
     <row r="10" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B10" s="6">
         <v>1600</v>
@@ -1627,7 +1621,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1654,7 +1648,7 @@
     </row>
     <row r="11" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B11" s="6">
         <v>1600</v>
@@ -1690,7 +1684,7 @@
     </row>
     <row r="12" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B12" s="6">
         <v>1600</v>
@@ -1735,7 +1729,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1771,7 +1765,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1807,7 +1801,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1870,7 +1864,7 @@
     </row>
     <row r="17" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B17" s="6">
         <v>1100</v>
@@ -1906,7 +1900,7 @@
     </row>
     <row r="18" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B18" s="6">
         <v>1100</v>
@@ -1942,7 +1936,7 @@
     </row>
     <row r="19" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B19" s="6">
         <v>1100</v>
@@ -1978,7 +1972,7 @@
     </row>
     <row r="20" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B20" s="6">
         <v>1100</v>
@@ -2014,7 +2008,7 @@
     </row>
     <row r="21" spans="1:26" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B21" s="6">
         <v>3700</v>
@@ -2050,7 +2044,7 @@
     </row>
     <row r="22" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B22" s="6">
         <v>3750</v>
@@ -2158,7 +2152,7 @@
     </row>
     <row r="25" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B25" s="6">
         <v>3250</v>
@@ -2194,7 +2188,7 @@
     </row>
     <row r="26" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B26" s="6">
         <v>4550</v>
@@ -2266,7 +2260,7 @@
     </row>
     <row r="28" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B28" s="6">
         <v>4850</v>
@@ -2383,7 +2377,7 @@
         <v>8</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -2416,10 +2410,10 @@
         <v>7100</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2482,7 +2476,7 @@
     </row>
     <row r="34" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B34" s="6">
         <v>7500</v>
@@ -2491,7 +2485,7 @@
         <v>5</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2518,7 +2512,7 @@
     </row>
     <row r="35" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B35" s="6">
         <v>7500</v>
@@ -2527,7 +2521,7 @@
         <v>8</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2554,7 +2548,7 @@
     </row>
     <row r="36" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B36" s="6">
         <v>1450</v>
@@ -2563,7 +2557,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2599,7 +2593,7 @@
         <v>5</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2635,7 +2629,7 @@
         <v>8</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2668,10 +2662,10 @@
         <v>2050</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2815,7 +2809,7 @@
         <v>5</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2851,7 +2845,7 @@
         <v>8</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2887,7 +2881,7 @@
         <v>9</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2959,7 +2953,7 @@
         <v>8</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2995,7 +2989,7 @@
         <v>12</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -3067,7 +3061,7 @@
         <v>5</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -3247,7 +3241,7 @@
         <v>6</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -3274,7 +3268,7 @@
     </row>
     <row r="56" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B56" s="6">
         <v>3050</v>
@@ -3310,7 +3304,7 @@
     </row>
     <row r="57" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B57" s="6">
         <v>4150</v>
@@ -3355,7 +3349,7 @@
         <v>5</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -3490,7 +3484,7 @@
     </row>
     <row r="62" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B62" s="6">
         <v>4250</v>
@@ -3535,7 +3529,7 @@
         <v>5</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -3562,7 +3556,7 @@
     </row>
     <row r="64" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B64" s="6">
         <v>4750</v>
@@ -3571,7 +3565,7 @@
         <v>5</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -3634,7 +3628,7 @@
     </row>
     <row r="66" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B66" s="6">
         <v>2250</v>
@@ -3670,7 +3664,7 @@
     </row>
     <row r="67" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B67" s="6">
         <v>2650</v>
@@ -3679,7 +3673,7 @@
         <v>5</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -3706,7 +3700,7 @@
     </row>
     <row r="68" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B68" s="6">
         <v>2650</v>
@@ -3715,7 +3709,7 @@
         <v>8</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -3931,7 +3925,7 @@
         <v>8</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -3967,7 +3961,7 @@
         <v>9</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -4039,7 +4033,7 @@
         <v>6</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -4075,7 +4069,7 @@
         <v>5</v>
       </c>
       <c r="D78" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
@@ -4108,10 +4102,10 @@
         <v>5700</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -4147,7 +4141,7 @@
         <v>5</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -4318,7 +4312,7 @@
     </row>
     <row r="85" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B85" s="6">
         <v>3850</v>
@@ -4354,7 +4348,7 @@
     </row>
     <row r="86" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B86" s="6">
         <v>4450</v>
@@ -4786,7 +4780,7 @@
     </row>
     <row r="98" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B98" s="6">
         <v>2950</v>
@@ -4930,7 +4924,7 @@
     </row>
     <row r="102" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B102" s="6">
         <v>3950</v>
@@ -4966,7 +4960,7 @@
     </row>
     <row r="103" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B103" s="6">
         <v>3550</v>
@@ -5002,7 +4996,7 @@
     </row>
     <row r="104" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B104" s="6">
         <v>3650</v>
@@ -5074,7 +5068,7 @@
     </row>
     <row r="106" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B106" s="6">
         <v>3450</v>
@@ -5110,7 +5104,7 @@
     </row>
     <row r="107" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B107" s="6">
         <v>3350</v>
@@ -5299,7 +5293,7 @@
         <v>6</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
@@ -5332,10 +5326,10 @@
         <v>1200</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
@@ -5506,7 +5500,7 @@
     </row>
     <row r="118" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B118" s="6">
         <v>2550</v>
@@ -5515,7 +5509,7 @@
         <v>5</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -5803,7 +5797,7 @@
         <v>6</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
@@ -5875,7 +5869,7 @@
         <v>8</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
@@ -5911,7 +5905,7 @@
         <v>12</v>
       </c>
       <c r="D129" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
@@ -5983,7 +5977,7 @@
         <v>8</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>119</v>
+        <v>214</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
@@ -6055,7 +6049,7 @@
         <v>9</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
@@ -6199,7 +6193,7 @@
         <v>9</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
@@ -6226,7 +6220,7 @@
     </row>
     <row r="138" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B138" s="6">
         <v>3150</v>
@@ -6235,7 +6229,7 @@
         <v>5</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -6262,7 +6256,7 @@
     </row>
     <row r="139" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B139" s="6">
         <v>3150</v>
@@ -6271,7 +6265,7 @@
         <v>8</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -6298,7 +6292,7 @@
     </row>
     <row r="140" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B140" s="6">
         <v>3150</v>
@@ -6307,7 +6301,7 @@
         <v>12</v>
       </c>
       <c r="D140" s="17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
@@ -6487,7 +6481,7 @@
         <v>8</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
@@ -6559,7 +6553,7 @@
         <v>12</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="148" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6573,7 +6567,7 @@
         <v>6</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="149" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6587,7 +6581,7 @@
         <v>5</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="150" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6601,7 +6595,7 @@
         <v>8</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="151" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6612,10 +6606,10 @@
         <v>7000</v>
       </c>
       <c r="C151" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D151" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="D151" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="152" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6643,7 +6637,7 @@
         <v>5</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="154" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6676,7 +6670,7 @@
     </row>
     <row r="156" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B156" s="6">
         <v>5510</v>
@@ -6690,7 +6684,7 @@
     </row>
     <row r="157" spans="1:26" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B157" s="6">
         <v>5520</v>
@@ -6726,7 +6720,7 @@
     </row>
     <row r="158" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B158" s="6">
         <v>7350</v>
@@ -6740,7 +6734,7 @@
     </row>
     <row r="159" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B159" s="6">
         <v>4400</v>
@@ -6749,12 +6743,12 @@
         <v>5</v>
       </c>
       <c r="D159" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="160" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A160" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B160" s="6">
         <v>4400</v>
@@ -6763,7 +6757,7 @@
         <v>8</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E160" s="1"/>
       <c r="F160" s="1"/>
@@ -6790,16 +6784,16 @@
     </row>
     <row r="161" spans="1:26" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A161" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B161" s="6">
         <v>4400</v>
       </c>
       <c r="C161" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="D161" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="D161" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="E161" s="1"/>
       <c r="F161" s="1"/>
@@ -6826,7 +6820,7 @@
     </row>
     <row r="162" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A162" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B162" s="6">
         <v>4400</v>
@@ -6835,7 +6829,7 @@
         <v>6</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E162" s="1"/>
       <c r="F162" s="1"/>
@@ -6862,7 +6856,7 @@
     </row>
     <row r="163" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A163" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B163" s="6">
         <v>5900</v>
@@ -6871,12 +6865,12 @@
         <v>5</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="164" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A164" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B164" s="6">
         <v>5900</v>
@@ -6885,12 +6879,12 @@
         <v>8</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="165" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A165" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B165" s="6">
         <v>5900</v>
@@ -6899,35 +6893,21 @@
         <v>12</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="166" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B166" s="6">
         <v>7200</v>
       </c>
-      <c r="C166" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D166" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="167" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A167" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="B167" s="6">
-        <v>7200</v>
-      </c>
-      <c r="C167" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D167" s="22" t="s">
-        <v>191</v>
+      <c r="C166" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D166" s="12">
+        <v>99999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>